<commit_message>
Zoom and pan working
alt-mousewheel will zoom the svg in and out, clicking and dragging will pan the body and the header around
</commit_message>
<xml_diff>
--- a/BigOlTimeline_Chart.xlsx
+++ b/BigOlTimeline_Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\Personal\BigOlTimeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2D404F-48D7-4FB2-9256-CF6D4BC2CC00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB123BB1-487E-4A61-A63F-927EBD5A3699}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Scotland</t>
   </si>
   <si>
-    <t>Britain</t>
-  </si>
-  <si>
     <t>Skandinavia</t>
   </si>
   <si>
@@ -60,12 +57,6 @@
     <t>France</t>
   </si>
   <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Italian Peninsula</t>
-  </si>
-  <si>
     <t>North Africa</t>
   </si>
   <si>
@@ -616,6 +607,15 @@
   </si>
   <si>
     <t>Romania: 1919-Present</t>
+  </si>
+  <si>
+    <t>Britannia</t>
+  </si>
+  <si>
+    <t>Hispania</t>
+  </si>
+  <si>
+    <t>Italia</t>
   </si>
 </sst>
 </file>
@@ -1461,20 +1461,8 @@
     <xf numFmtId="0" fontId="0" fillId="51" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1483,96 +1471,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1665,6 +1563,63 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1707,7 +1662,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1741,6 +1720,54 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1761,6 +1788,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1773,99 +1884,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1875,6 +1893,54 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1905,28 +1971,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1953,48 +2013,6 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="48" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="48" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="48" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="49" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2020,24 +2038,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="52" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2336,8 +2336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7CFCAE-E1AA-4E44-87FB-807FA0F08CCC}">
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56:I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2353,132 +2353,132 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3800</v>
       </c>
-      <c r="B2" s="55" t="s">
-        <v>41</v>
+      <c r="B2" s="51" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2498,8 +2498,8 @@
       <c r="R2" s="1"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
-      <c r="U2" s="88" t="s">
-        <v>60</v>
+      <c r="U2" s="54" t="s">
+        <v>57</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
@@ -2529,7 +2529,7 @@
       <c r="A3" s="1">
         <v>3700</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2548,7 +2548,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="89"/>
+      <c r="U3" s="55"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -2577,7 +2577,7 @@
       <c r="A4" s="1">
         <v>3600</v>
       </c>
-      <c r="B4" s="56"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2596,7 +2596,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="89"/>
+      <c r="U4" s="55"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -2625,7 +2625,7 @@
       <c r="A5" s="1">
         <v>3500</v>
       </c>
-      <c r="B5" s="56"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2644,7 +2644,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
-      <c r="U5" s="89"/>
+      <c r="U5" s="55"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
@@ -2673,7 +2673,7 @@
       <c r="A6" s="1">
         <v>3400</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2692,7 +2692,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-      <c r="U6" s="89"/>
+      <c r="U6" s="55"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -2721,8 +2721,8 @@
       <c r="A7" s="1">
         <v>3300</v>
       </c>
-      <c r="B7" s="91" t="s">
-        <v>61</v>
+      <c r="B7" s="57" t="s">
+        <v>58</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2742,7 +2742,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="89"/>
+      <c r="U7" s="55"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
@@ -2771,7 +2771,7 @@
       <c r="A8" s="1">
         <v>3200</v>
       </c>
-      <c r="B8" s="92"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2790,7 +2790,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
-      <c r="U8" s="89"/>
+      <c r="U8" s="55"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -2819,7 +2819,7 @@
       <c r="A9" s="1">
         <v>3100</v>
       </c>
-      <c r="B9" s="92"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2836,11 +2836,11 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="94" t="s">
-        <v>62</v>
+      <c r="S9" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="T9" s="3"/>
-      <c r="U9" s="89"/>
+      <c r="U9" s="55"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
@@ -2869,7 +2869,7 @@
       <c r="A10" s="1">
         <v>3000</v>
       </c>
-      <c r="B10" s="92"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2886,9 +2886,9 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="95"/>
+      <c r="S10" s="61"/>
       <c r="T10" s="3"/>
-      <c r="U10" s="89"/>
+      <c r="U10" s="55"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
@@ -2917,7 +2917,7 @@
       <c r="A11" s="1">
         <v>2900</v>
       </c>
-      <c r="B11" s="92"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2934,9 +2934,9 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="95"/>
+      <c r="S11" s="61"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="89"/>
+      <c r="U11" s="55"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
@@ -2965,7 +2965,7 @@
       <c r="A12" s="1">
         <v>2800</v>
       </c>
-      <c r="B12" s="92"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2982,9 +2982,9 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="95"/>
+      <c r="S12" s="61"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="89"/>
+      <c r="U12" s="55"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -3013,7 +3013,7 @@
       <c r="A13" s="1">
         <v>2700</v>
       </c>
-      <c r="B13" s="92"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -3030,9 +3030,9 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="95"/>
+      <c r="S13" s="61"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="89"/>
+      <c r="U13" s="55"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -3061,7 +3061,7 @@
       <c r="A14" s="1">
         <v>2600</v>
       </c>
-      <c r="B14" s="92"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3078,9 +3078,9 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
-      <c r="S14" s="95"/>
+      <c r="S14" s="61"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="89"/>
+      <c r="U14" s="55"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -3109,7 +3109,7 @@
       <c r="A15" s="1">
         <v>2500</v>
       </c>
-      <c r="B15" s="92"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -3126,11 +3126,11 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="95" t="s">
-        <v>63</v>
+      <c r="S15" s="61" t="s">
+        <v>60</v>
       </c>
       <c r="T15" s="3"/>
-      <c r="U15" s="89"/>
+      <c r="U15" s="55"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
@@ -3159,7 +3159,7 @@
       <c r="A16" s="1">
         <v>2400</v>
       </c>
-      <c r="B16" s="92"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -3176,9 +3176,9 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="95"/>
+      <c r="S16" s="61"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="89"/>
+      <c r="U16" s="55"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
@@ -3207,7 +3207,7 @@
       <c r="A17" s="1">
         <v>2300</v>
       </c>
-      <c r="B17" s="92"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -3224,9 +3224,9 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="95"/>
+      <c r="S17" s="61"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="90"/>
+      <c r="U17" s="56"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -3255,7 +3255,7 @@
       <c r="A18" s="1">
         <v>2200</v>
       </c>
-      <c r="B18" s="92"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3272,10 +3272,10 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="95"/>
+      <c r="S18" s="61"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="96" t="s">
-        <v>64</v>
+      <c r="U18" s="62" t="s">
+        <v>61</v>
       </c>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
@@ -3305,7 +3305,7 @@
       <c r="A19" s="1">
         <v>2100</v>
       </c>
-      <c r="B19" s="92"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3323,10 +3323,10 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="T19" s="3"/>
-      <c r="U19" s="97"/>
+      <c r="U19" s="63"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
@@ -3355,7 +3355,7 @@
       <c r="A20" s="1">
         <v>2000</v>
       </c>
-      <c r="B20" s="92"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -3372,8 +3372,8 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-      <c r="S20" s="98" t="s">
-        <v>66</v>
+      <c r="S20" s="64" t="s">
+        <v>63</v>
       </c>
       <c r="T20" s="28"/>
       <c r="U20" s="1"/>
@@ -3405,7 +3405,7 @@
       <c r="A21" s="1">
         <v>1900</v>
       </c>
-      <c r="B21" s="92"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -3422,10 +3422,10 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="98"/>
+      <c r="S21" s="64"/>
       <c r="T21" s="28"/>
-      <c r="U21" s="99" t="s">
-        <v>67</v>
+      <c r="U21" s="65" t="s">
+        <v>64</v>
       </c>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
@@ -3455,7 +3455,7 @@
       <c r="A22" s="1">
         <v>1800</v>
       </c>
-      <c r="B22" s="92"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -3472,11 +3472,11 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="98"/>
+      <c r="S22" s="64"/>
       <c r="T22" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="U22" s="100"/>
+        <v>65</v>
+      </c>
+      <c r="U22" s="66"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
@@ -3505,7 +3505,7 @@
       <c r="A23" s="1">
         <v>1700</v>
       </c>
-      <c r="B23" s="92"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -3522,7 +3522,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-      <c r="S23" s="98"/>
+      <c r="S23" s="64"/>
       <c r="T23" s="28"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
@@ -3553,7 +3553,7 @@
       <c r="A24" s="1">
         <v>1600</v>
       </c>
-      <c r="B24" s="92"/>
+      <c r="B24" s="58"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -3569,13 +3569,13 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="101" t="s">
-        <v>69</v>
-      </c>
-      <c r="S24" s="98"/>
+      <c r="R24" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="S24" s="64"/>
       <c r="T24" s="28"/>
-      <c r="U24" s="104" t="s">
-        <v>70</v>
+      <c r="U24" s="70" t="s">
+        <v>67</v>
       </c>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
@@ -3605,7 +3605,7 @@
       <c r="A25" s="1">
         <v>1500</v>
       </c>
-      <c r="B25" s="92"/>
+      <c r="B25" s="58"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -3621,12 +3621,12 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="102"/>
+      <c r="R25" s="68"/>
       <c r="S25" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="T25" s="3"/>
-      <c r="U25" s="105"/>
+      <c r="U25" s="71"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -3655,7 +3655,7 @@
       <c r="A26" s="1">
         <v>1400</v>
       </c>
-      <c r="B26" s="92"/>
+      <c r="B26" s="58"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -3671,12 +3671,12 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="102"/>
-      <c r="S26" s="98" t="s">
-        <v>72</v>
-      </c>
-      <c r="T26" s="106" t="s">
-        <v>73</v>
+      <c r="R26" s="68"/>
+      <c r="S26" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="T26" s="72" t="s">
+        <v>70</v>
       </c>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
@@ -3707,7 +3707,7 @@
       <c r="A27" s="1">
         <v>1300</v>
       </c>
-      <c r="B27" s="92"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -3723,9 +3723,9 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="102"/>
-      <c r="S27" s="98"/>
-      <c r="T27" s="107"/>
+      <c r="R27" s="68"/>
+      <c r="S27" s="64"/>
+      <c r="T27" s="73"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
@@ -3755,7 +3755,7 @@
       <c r="A28" s="1">
         <v>1200</v>
       </c>
-      <c r="B28" s="93"/>
+      <c r="B28" s="59"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -3771,9 +3771,9 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="103"/>
-      <c r="S28" s="98"/>
-      <c r="T28" s="108"/>
+      <c r="R28" s="69"/>
+      <c r="S28" s="64"/>
+      <c r="T28" s="74"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
@@ -3803,8 +3803,8 @@
       <c r="A29" s="1">
         <v>1100</v>
       </c>
-      <c r="B29" s="109" t="s">
-        <v>56</v>
+      <c r="B29" s="75" t="s">
+        <v>53</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -3821,10 +3821,10 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="112" t="s">
-        <v>74</v>
-      </c>
-      <c r="S29" s="98"/>
+      <c r="R29" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="S29" s="64"/>
       <c r="T29" s="28"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
@@ -3855,7 +3855,7 @@
       <c r="A30" s="1">
         <v>1000</v>
       </c>
-      <c r="B30" s="110"/>
+      <c r="B30" s="76"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -3871,8 +3871,8 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="113"/>
-      <c r="S30" s="98"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="64"/>
       <c r="T30" s="28"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
@@ -3903,7 +3903,7 @@
       <c r="A31" s="1">
         <v>900</v>
       </c>
-      <c r="B31" s="110"/>
+      <c r="B31" s="76"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -3919,12 +3919,12 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
-      <c r="R31" s="113"/>
-      <c r="S31" s="115" t="s">
-        <v>75</v>
+      <c r="R31" s="79"/>
+      <c r="S31" s="81" t="s">
+        <v>72</v>
       </c>
       <c r="T31" s="14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
@@ -3955,7 +3955,7 @@
       <c r="A32" s="1">
         <v>800</v>
       </c>
-      <c r="B32" s="110"/>
+      <c r="B32" s="76"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -3971,8 +3971,8 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="113"/>
-      <c r="S32" s="115"/>
+      <c r="R32" s="79"/>
+      <c r="S32" s="81"/>
       <c r="T32" s="28"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
@@ -4003,7 +4003,7 @@
       <c r="A33" s="1">
         <v>700</v>
       </c>
-      <c r="B33" s="110"/>
+      <c r="B33" s="76"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -4014,18 +4014,18 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="116" t="s">
-        <v>77</v>
+      <c r="M33" s="82" t="s">
+        <v>74</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="114"/>
-      <c r="S33" s="115"/>
+      <c r="R33" s="80"/>
+      <c r="S33" s="81"/>
       <c r="T33" s="33"/>
-      <c r="U33" s="70" t="s">
-        <v>78</v>
+      <c r="U33" s="84" t="s">
+        <v>75</v>
       </c>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
@@ -4055,7 +4055,7 @@
       <c r="A34" s="1">
         <v>600</v>
       </c>
-      <c r="B34" s="110"/>
+      <c r="B34" s="76"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -4066,23 +4066,23 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-      <c r="M34" s="117"/>
-      <c r="N34" s="72" t="s">
-        <v>79</v>
+      <c r="M34" s="83"/>
+      <c r="N34" s="86" t="s">
+        <v>76</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
-      <c r="Q34" s="75" t="s">
-        <v>80</v>
-      </c>
-      <c r="R34" s="76"/>
+      <c r="Q34" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="R34" s="90"/>
       <c r="S34" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="U34" s="71"/>
+        <v>79</v>
+      </c>
+      <c r="U34" s="85"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
@@ -4111,7 +4111,7 @@
       <c r="A35" s="1">
         <v>500</v>
       </c>
-      <c r="B35" s="111"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -4122,24 +4122,24 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="117"/>
-      <c r="N35" s="73"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="87"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-      <c r="Q35" s="77"/>
-      <c r="R35" s="78"/>
+      <c r="Q35" s="91"/>
+      <c r="R35" s="92"/>
       <c r="S35" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="T35" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="U35" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V35" s="1"/>
       <c r="W35" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
@@ -4167,8 +4167,8 @@
       <c r="A36" s="1">
         <v>400</v>
       </c>
-      <c r="B36" s="79" t="s">
-        <v>57</v>
+      <c r="B36" s="93" t="s">
+        <v>54</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -4180,32 +4180,32 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="N36" s="73"/>
+      <c r="M36" s="96" t="s">
+        <v>84</v>
+      </c>
+      <c r="N36" s="87"/>
       <c r="O36" s="1"/>
       <c r="P36" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q36" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="R36" s="98"/>
+      <c r="S36" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="T36" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="Q36" s="84" t="s">
+      <c r="U36" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="R36" s="84"/>
-      <c r="S36" s="42" t="s">
+      <c r="V36" s="1"/>
+      <c r="W36" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="T36" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="U36" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="V36" s="1"/>
-      <c r="W36" s="118" t="s">
-        <v>93</v>
-      </c>
-      <c r="X36" s="119"/>
+      <c r="X36" s="104"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
@@ -4231,7 +4231,7 @@
       <c r="A37" s="1">
         <v>300</v>
       </c>
-      <c r="B37" s="80"/>
+      <c r="B37" s="94"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -4242,33 +4242,33 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
-      <c r="M37" s="82"/>
-      <c r="N37" s="73"/>
+      <c r="M37" s="96"/>
+      <c r="N37" s="87"/>
       <c r="O37" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="P37" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q37" s="105" t="s">
+        <v>93</v>
+      </c>
+      <c r="R37" s="106"/>
+      <c r="S37" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="P37" s="39" t="s">
+      <c r="T37" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="Q37" s="120" t="s">
+      <c r="U37" s="40" t="s">
         <v>96</v>
-      </c>
-      <c r="R37" s="121"/>
-      <c r="S37" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="T37" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="U37" s="40" t="s">
-        <v>99</v>
       </c>
       <c r="V37" s="1"/>
       <c r="W37" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="X37" s="40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
@@ -4295,7 +4295,7 @@
       <c r="A38" s="1">
         <v>200</v>
       </c>
-      <c r="B38" s="80"/>
+      <c r="B38" s="94"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -4306,20 +4306,20 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="82"/>
-      <c r="N38" s="74"/>
+      <c r="M38" s="96"/>
+      <c r="N38" s="88"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="S38" s="122" t="s">
-        <v>103</v>
+        <v>99</v>
+      </c>
+      <c r="S38" s="107" t="s">
+        <v>100</v>
       </c>
       <c r="T38" s="1"/>
-      <c r="U38" s="125" t="s">
-        <v>104</v>
+      <c r="U38" s="110" t="s">
+        <v>101</v>
       </c>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
@@ -4349,7 +4349,7 @@
       <c r="A39" s="1">
         <v>100</v>
       </c>
-      <c r="B39" s="80"/>
+      <c r="B39" s="94"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -4359,26 +4359,26 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="36"/>
-      <c r="L39" s="85" t="s">
-        <v>105</v>
-      </c>
-      <c r="M39" s="83"/>
+      <c r="L39" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="M39" s="97"/>
       <c r="N39" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="O39" s="85" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="O39" s="99" t="s">
+        <v>104</v>
       </c>
       <c r="P39" s="28"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="123"/>
+      <c r="S39" s="108"/>
       <c r="T39" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="U39" s="126"/>
-      <c r="W39" s="127" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="U39" s="111"/>
+      <c r="W39" s="112" t="s">
+        <v>106</v>
       </c>
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
@@ -4406,7 +4406,7 @@
       <c r="A40" s="1">
         <v>0</v>
       </c>
-      <c r="B40" s="80"/>
+      <c r="B40" s="94"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -4415,26 +4415,26 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="36"/>
-      <c r="K40" s="85" t="s">
-        <v>110</v>
-      </c>
-      <c r="L40" s="86"/>
-      <c r="M40" s="83"/>
+      <c r="K40" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="L40" s="100"/>
+      <c r="M40" s="97"/>
       <c r="N40" s="38"/>
-      <c r="O40" s="86"/>
+      <c r="O40" s="100"/>
       <c r="P40" s="34"/>
-      <c r="Q40" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="R40" s="85"/>
-      <c r="S40" s="124"/>
-      <c r="T40" s="130" t="s">
-        <v>111</v>
-      </c>
-      <c r="U40" s="127" t="s">
-        <v>112</v>
-      </c>
-      <c r="W40" s="128"/>
+      <c r="Q40" s="99" t="s">
+        <v>108</v>
+      </c>
+      <c r="R40" s="99"/>
+      <c r="S40" s="109"/>
+      <c r="T40" s="115" t="s">
+        <v>108</v>
+      </c>
+      <c r="U40" s="112" t="s">
+        <v>109</v>
+      </c>
+      <c r="W40" s="113"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
@@ -4461,7 +4461,7 @@
       <c r="A41" s="1">
         <v>100</v>
       </c>
-      <c r="B41" s="80"/>
+      <c r="B41" s="94"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -4470,26 +4470,26 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="K41" s="100"/>
+      <c r="L41" s="100"/>
+      <c r="M41" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="N41" s="99" t="s">
+        <v>112</v>
+      </c>
+      <c r="O41" s="100"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="100"/>
+      <c r="R41" s="100"/>
+      <c r="S41" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="K41" s="86"/>
-      <c r="L41" s="86"/>
-      <c r="M41" s="86" t="s">
-        <v>114</v>
-      </c>
-      <c r="N41" s="85" t="s">
-        <v>115</v>
-      </c>
-      <c r="O41" s="86"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="86"/>
-      <c r="S41" s="85" t="s">
-        <v>116</v>
-      </c>
-      <c r="T41" s="83"/>
-      <c r="U41" s="128"/>
-      <c r="W41" s="128"/>
+      <c r="T41" s="97"/>
+      <c r="U41" s="113"/>
+      <c r="W41" s="113"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
@@ -4504,13 +4504,13 @@
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL41" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM41" s="59"/>
-      <c r="AN41" s="60"/>
+        <v>39</v>
+      </c>
+      <c r="AL41" s="117" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM41" s="118"/>
+      <c r="AN41" s="119"/>
       <c r="AO41" s="1"/>
       <c r="AP41" s="1"/>
       <c r="AQ41" s="1"/>
@@ -4520,31 +4520,31 @@
       <c r="A42" s="1">
         <v>200</v>
       </c>
-      <c r="B42" s="80"/>
+      <c r="B42" s="94"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="130" t="s">
-        <v>117</v>
+      <c r="E42" s="115" t="s">
+        <v>114</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="35"/>
-      <c r="K42" s="86"/>
-      <c r="L42" s="86"/>
-      <c r="M42" s="86"/>
-      <c r="N42" s="86"/>
-      <c r="O42" s="86"/>
-      <c r="P42" s="86" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q42" s="86"/>
-      <c r="R42" s="86"/>
-      <c r="S42" s="86"/>
-      <c r="T42" s="83"/>
-      <c r="U42" s="129"/>
-      <c r="W42" s="129"/>
+      <c r="K42" s="100"/>
+      <c r="L42" s="100"/>
+      <c r="M42" s="100"/>
+      <c r="N42" s="100"/>
+      <c r="O42" s="100"/>
+      <c r="P42" s="100" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q42" s="100"/>
+      <c r="R42" s="100"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="97"/>
+      <c r="U42" s="114"/>
+      <c r="W42" s="114"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
@@ -4559,11 +4559,11 @@
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL42" s="61"/>
-      <c r="AM42" s="62"/>
-      <c r="AN42" s="63"/>
+        <v>41</v>
+      </c>
+      <c r="AL42" s="120"/>
+      <c r="AM42" s="121"/>
+      <c r="AN42" s="122"/>
       <c r="AO42" s="1"/>
       <c r="AP42" s="1"/>
       <c r="AQ42" s="1"/>
@@ -4573,31 +4573,31 @@
       <c r="A43" s="1">
         <v>300</v>
       </c>
-      <c r="B43" s="80"/>
+      <c r="B43" s="94"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="82"/>
+      <c r="E43" s="96"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="7"/>
-      <c r="K43" s="86"/>
-      <c r="L43" s="86"/>
-      <c r="M43" s="86"/>
-      <c r="N43" s="86"/>
-      <c r="O43" s="86"/>
-      <c r="P43" s="86"/>
-      <c r="Q43" s="86"/>
-      <c r="R43" s="86"/>
-      <c r="S43" s="86"/>
-      <c r="T43" s="83"/>
-      <c r="U43" s="134" t="s">
-        <v>119</v>
-      </c>
-      <c r="V43" s="239"/>
-      <c r="W43" s="99" t="s">
-        <v>120</v>
+      <c r="K43" s="100"/>
+      <c r="L43" s="100"/>
+      <c r="M43" s="100"/>
+      <c r="N43" s="100"/>
+      <c r="O43" s="100"/>
+      <c r="P43" s="100"/>
+      <c r="Q43" s="100"/>
+      <c r="R43" s="100"/>
+      <c r="S43" s="100"/>
+      <c r="T43" s="97"/>
+      <c r="U43" s="127" t="s">
+        <v>116</v>
+      </c>
+      <c r="V43" s="50"/>
+      <c r="W43" s="65" t="s">
+        <v>117</v>
       </c>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
@@ -4613,11 +4613,11 @@
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AL43" s="61"/>
-      <c r="AM43" s="62"/>
-      <c r="AN43" s="63"/>
+        <v>42</v>
+      </c>
+      <c r="AL43" s="120"/>
+      <c r="AM43" s="121"/>
+      <c r="AN43" s="122"/>
       <c r="AO43" s="1"/>
       <c r="AP43" s="1"/>
       <c r="AQ43" s="1"/>
@@ -4627,28 +4627,28 @@
       <c r="A44" s="1">
         <v>400</v>
       </c>
-      <c r="B44" s="80"/>
+      <c r="B44" s="94"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="133"/>
+      <c r="E44" s="126"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="7"/>
-      <c r="K44" s="86"/>
-      <c r="L44" s="86"/>
-      <c r="M44" s="86"/>
-      <c r="N44" s="87"/>
-      <c r="O44" s="87"/>
-      <c r="P44" s="87"/>
-      <c r="Q44" s="87"/>
-      <c r="R44" s="87"/>
-      <c r="S44" s="87"/>
-      <c r="T44" s="131"/>
-      <c r="U44" s="135"/>
-      <c r="V44" s="239"/>
-      <c r="W44" s="137"/>
+      <c r="K44" s="100"/>
+      <c r="L44" s="100"/>
+      <c r="M44" s="100"/>
+      <c r="N44" s="101"/>
+      <c r="O44" s="101"/>
+      <c r="P44" s="101"/>
+      <c r="Q44" s="101"/>
+      <c r="R44" s="101"/>
+      <c r="S44" s="101"/>
+      <c r="T44" s="116"/>
+      <c r="U44" s="128"/>
+      <c r="V44" s="50"/>
+      <c r="W44" s="130"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
@@ -4663,11 +4663,11 @@
       <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL44" s="64"/>
-      <c r="AM44" s="65"/>
-      <c r="AN44" s="66"/>
+        <v>43</v>
+      </c>
+      <c r="AL44" s="123"/>
+      <c r="AM44" s="124"/>
+      <c r="AN44" s="125"/>
       <c r="AO44" s="1"/>
       <c r="AP44" s="1"/>
       <c r="AQ44" s="1"/>
@@ -4677,7 +4677,7 @@
       <c r="A45" s="1">
         <v>500</v>
       </c>
-      <c r="B45" s="81"/>
+      <c r="B45" s="95"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -4686,31 +4686,31 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="7"/>
-      <c r="K45" s="87"/>
-      <c r="L45" s="87"/>
-      <c r="M45" s="132"/>
+      <c r="K45" s="101"/>
+      <c r="L45" s="101"/>
+      <c r="M45" s="102"/>
       <c r="N45" s="32"/>
-      <c r="O45" s="139" t="s">
+      <c r="O45" s="132" t="s">
+        <v>118</v>
+      </c>
+      <c r="P45" s="132" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q45" s="132" t="s">
+        <v>120</v>
+      </c>
+      <c r="R45" s="132" t="s">
         <v>121</v>
       </c>
-      <c r="P45" s="139" t="s">
+      <c r="S45" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="Q45" s="139" t="s">
+      <c r="T45" s="135" t="s">
         <v>123</v>
       </c>
-      <c r="R45" s="139" t="s">
-        <v>124</v>
-      </c>
-      <c r="S45" s="139" t="s">
-        <v>125</v>
-      </c>
-      <c r="T45" s="142" t="s">
-        <v>126</v>
-      </c>
-      <c r="U45" s="135"/>
-      <c r="V45" s="239"/>
-      <c r="W45" s="137"/>
+      <c r="U45" s="128"/>
+      <c r="V45" s="50"/>
+      <c r="W45" s="130"/>
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
@@ -4725,10 +4725,10 @@
       <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AL45" s="67" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="AL45" s="137" t="s">
+        <v>45</v>
       </c>
       <c r="AM45" s="1"/>
       <c r="AN45" s="1"/>
@@ -4741,8 +4741,8 @@
       <c r="A46" s="1">
         <v>600</v>
       </c>
-      <c r="B46" s="154" t="s">
-        <v>58</v>
+      <c r="B46" s="140" t="s">
+        <v>55</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -4750,29 +4750,29 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="157" t="s">
-        <v>127</v>
+      <c r="I46" s="143" t="s">
+        <v>124</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="160" t="s">
-        <v>128</v>
+      <c r="L46" s="146" t="s">
+        <v>125</v>
       </c>
       <c r="M46" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="N46" s="162" t="s">
-        <v>130</v>
-      </c>
-      <c r="O46" s="140"/>
-      <c r="P46" s="140"/>
-      <c r="Q46" s="140"/>
-      <c r="R46" s="141"/>
-      <c r="S46" s="141"/>
-      <c r="T46" s="143"/>
-      <c r="U46" s="135"/>
-      <c r="V46" s="239"/>
-      <c r="W46" s="137"/>
+        <v>126</v>
+      </c>
+      <c r="N46" s="148" t="s">
+        <v>127</v>
+      </c>
+      <c r="O46" s="133"/>
+      <c r="P46" s="133"/>
+      <c r="Q46" s="133"/>
+      <c r="R46" s="134"/>
+      <c r="S46" s="134"/>
+      <c r="T46" s="136"/>
+      <c r="U46" s="128"/>
+      <c r="V46" s="50"/>
+      <c r="W46" s="130"/>
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
@@ -4787,7 +4787,7 @@
       <c r="AI46" s="1"/>
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
-      <c r="AL46" s="68"/>
+      <c r="AL46" s="138"/>
       <c r="AM46" s="1"/>
       <c r="AN46" s="1"/>
       <c r="AO46" s="1"/>
@@ -4799,40 +4799,40 @@
       <c r="A47" s="1">
         <v>700</v>
       </c>
-      <c r="B47" s="155"/>
+      <c r="B47" s="141"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="158"/>
+      <c r="I47" s="144"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="164" t="s">
+      <c r="K47" s="150" t="s">
+        <v>128</v>
+      </c>
+      <c r="L47" s="147"/>
+      <c r="M47" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="N47" s="149"/>
+      <c r="O47" s="133"/>
+      <c r="P47" s="133"/>
+      <c r="Q47" s="133"/>
+      <c r="R47" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="S47" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="L47" s="161"/>
-      <c r="M47" s="23" t="s">
+      <c r="T47" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="N47" s="163"/>
-      <c r="O47" s="140"/>
-      <c r="P47" s="140"/>
-      <c r="Q47" s="140"/>
-      <c r="R47" s="29" t="s">
+      <c r="U47" s="129"/>
+      <c r="V47" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="S47" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="T47" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="U47" s="136"/>
-      <c r="V47" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="W47" s="138"/>
+      <c r="W47" s="131"/>
       <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
@@ -4847,7 +4847,7 @@
       <c r="AI47" s="1"/>
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
-      <c r="AL47" s="68"/>
+      <c r="AL47" s="138"/>
       <c r="AM47" s="1"/>
       <c r="AN47" s="1"/>
       <c r="AO47" s="1"/>
@@ -4859,32 +4859,32 @@
       <c r="A48" s="1">
         <v>800</v>
       </c>
-      <c r="B48" s="155"/>
+      <c r="B48" s="141"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="159"/>
+      <c r="I48" s="145"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="165"/>
+      <c r="K48" s="151"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-      <c r="O48" s="140"/>
-      <c r="P48" s="140"/>
-      <c r="Q48" s="140"/>
-      <c r="R48" s="144" t="s">
-        <v>137</v>
-      </c>
-      <c r="S48" s="147" t="s">
-        <v>138</v>
-      </c>
-      <c r="T48" s="148"/>
-      <c r="U48" s="148"/>
-      <c r="V48" s="148"/>
-      <c r="W48" s="149"/>
+      <c r="O48" s="133"/>
+      <c r="P48" s="133"/>
+      <c r="Q48" s="133"/>
+      <c r="R48" s="153" t="s">
+        <v>134</v>
+      </c>
+      <c r="S48" s="156" t="s">
+        <v>135</v>
+      </c>
+      <c r="T48" s="157"/>
+      <c r="U48" s="157"/>
+      <c r="V48" s="157"/>
+      <c r="W48" s="158"/>
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
@@ -4899,7 +4899,7 @@
       <c r="AI48" s="1"/>
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
-      <c r="AL48" s="68"/>
+      <c r="AL48" s="138"/>
       <c r="AM48" s="1"/>
       <c r="AN48" s="1"/>
       <c r="AO48" s="1"/>
@@ -4911,39 +4911,39 @@
       <c r="A49" s="1">
         <v>900</v>
       </c>
-      <c r="B49" s="155"/>
+      <c r="B49" s="141"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="167" t="s">
-        <v>139</v>
+      <c r="D49" s="159" t="s">
+        <v>136</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="170" t="s">
-        <v>140</v>
+      <c r="G49" s="184" t="s">
+        <v>137</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J49" s="1"/>
-      <c r="K49" s="166"/>
+      <c r="K49" s="152"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="O49" s="140"/>
-      <c r="P49" s="140"/>
-      <c r="Q49" s="140"/>
-      <c r="R49" s="145"/>
+      <c r="O49" s="133"/>
+      <c r="P49" s="133"/>
+      <c r="Q49" s="133"/>
+      <c r="R49" s="154"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
-      <c r="U49" s="150" t="s">
-        <v>142</v>
-      </c>
-      <c r="V49" s="152" t="s">
-        <v>143</v>
+      <c r="U49" s="187" t="s">
+        <v>139</v>
+      </c>
+      <c r="V49" s="189" t="s">
+        <v>140</v>
       </c>
       <c r="W49" s="36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="X49" s="1"/>
       <c r="Y49" s="1"/>
@@ -4959,7 +4959,7 @@
       <c r="AI49" s="1"/>
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
-      <c r="AL49" s="68"/>
+      <c r="AL49" s="138"/>
       <c r="AM49" s="1"/>
       <c r="AN49" s="1"/>
       <c r="AO49" s="1"/>
@@ -4971,35 +4971,35 @@
       <c r="A50" s="1">
         <v>1000</v>
       </c>
-      <c r="B50" s="155"/>
+      <c r="B50" s="141"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="168"/>
-      <c r="E50" s="173" t="s">
-        <v>145</v>
+      <c r="D50" s="160"/>
+      <c r="E50" s="162" t="s">
+        <v>142</v>
       </c>
       <c r="F50" s="1"/>
-      <c r="G50" s="171"/>
-      <c r="H50" s="176" t="s">
-        <v>146</v>
+      <c r="G50" s="185"/>
+      <c r="H50" s="165" t="s">
+        <v>143</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-      <c r="O50" s="140"/>
-      <c r="P50" s="140"/>
-      <c r="Q50" s="140"/>
-      <c r="R50" s="145"/>
+      <c r="O50" s="133"/>
+      <c r="P50" s="133"/>
+      <c r="Q50" s="133"/>
+      <c r="R50" s="154"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
-      <c r="U50" s="151"/>
-      <c r="V50" s="153"/>
+      <c r="U50" s="188"/>
+      <c r="V50" s="190"/>
       <c r="W50" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="X50" s="1"/>
       <c r="Y50" s="1"/>
@@ -5015,7 +5015,7 @@
       <c r="AI50" s="1"/>
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
-      <c r="AL50" s="68"/>
+      <c r="AL50" s="138"/>
       <c r="AM50" s="1"/>
       <c r="AN50" s="1"/>
       <c r="AO50" s="1"/>
@@ -5027,39 +5027,39 @@
       <c r="A51" s="1">
         <v>1100</v>
       </c>
-      <c r="B51" s="155"/>
+      <c r="B51" s="141"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="168"/>
-      <c r="E51" s="174"/>
+      <c r="D51" s="160"/>
+      <c r="E51" s="163"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="172"/>
-      <c r="H51" s="177"/>
+      <c r="G51" s="186"/>
+      <c r="H51" s="166"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="179" t="s">
-        <v>149</v>
-      </c>
-      <c r="K51" s="182" t="s">
-        <v>150</v>
+      <c r="J51" s="168" t="s">
+        <v>146</v>
+      </c>
+      <c r="K51" s="171" t="s">
+        <v>147</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
-      <c r="O51" s="140"/>
-      <c r="P51" s="140"/>
-      <c r="Q51" s="140"/>
-      <c r="R51" s="146"/>
+      <c r="O51" s="133"/>
+      <c r="P51" s="133"/>
+      <c r="Q51" s="133"/>
+      <c r="R51" s="155"/>
       <c r="S51" s="1"/>
       <c r="T51" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="U51" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="V51" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="W51" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="U51" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="V51" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="W51" s="16" t="s">
-        <v>154</v>
       </c>
       <c r="X51" s="1"/>
       <c r="Y51" s="1"/>
@@ -5074,10 +5074,10 @@
       <c r="AH51" s="1"/>
       <c r="AI51" s="1"/>
       <c r="AJ51" s="1"/>
-      <c r="AK51" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL51" s="68"/>
+      <c r="AK51" s="207" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL51" s="138"/>
       <c r="AM51" s="1"/>
       <c r="AN51" s="1"/>
       <c r="AO51" s="1"/>
@@ -5089,32 +5089,32 @@
       <c r="A52" s="1">
         <v>1200</v>
       </c>
-      <c r="B52" s="155"/>
+      <c r="B52" s="141"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="168"/>
-      <c r="E52" s="174"/>
+      <c r="D52" s="160"/>
+      <c r="E52" s="163"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="177"/>
+      <c r="H52" s="166"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="180"/>
-      <c r="K52" s="183"/>
+      <c r="J52" s="169"/>
+      <c r="K52" s="172"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
-      <c r="O52" s="141"/>
-      <c r="P52" s="141"/>
-      <c r="Q52" s="140"/>
+      <c r="O52" s="134"/>
+      <c r="P52" s="134"/>
+      <c r="Q52" s="133"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W52" s="1"/>
       <c r="X52" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
@@ -5127,11 +5127,11 @@
       <c r="AG52" s="1"/>
       <c r="AH52" s="1"/>
       <c r="AI52" s="1"/>
-      <c r="AJ52" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK52" s="53"/>
-      <c r="AL52" s="68"/>
+      <c r="AJ52" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK52" s="208"/>
+      <c r="AL52" s="138"/>
       <c r="AM52" s="1"/>
       <c r="AN52" s="1"/>
       <c r="AO52" s="1"/>
@@ -5143,42 +5143,42 @@
       <c r="A53" s="1">
         <v>1300</v>
       </c>
-      <c r="B53" s="155"/>
-      <c r="C53" s="188" t="s">
-        <v>157</v>
-      </c>
-      <c r="D53" s="168"/>
-      <c r="E53" s="174"/>
+      <c r="B53" s="141"/>
+      <c r="C53" s="210" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" s="160"/>
+      <c r="E53" s="163"/>
       <c r="F53" s="1"/>
       <c r="G53" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="H53" s="177"/>
+        <v>155</v>
+      </c>
+      <c r="H53" s="166"/>
       <c r="I53" s="1"/>
-      <c r="J53" s="180"/>
-      <c r="K53" s="183"/>
+      <c r="J53" s="169"/>
+      <c r="K53" s="172"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
-      <c r="Q53" s="140"/>
+      <c r="Q53" s="133"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
       <c r="T53" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="U53" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="V53" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="W53" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="U53" s="16" t="s">
+      <c r="X53" s="16" t="s">
         <v>160</v>
-      </c>
-      <c r="V53" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="W53" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="X53" s="16" t="s">
-        <v>163</v>
       </c>
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
@@ -5191,9 +5191,9 @@
       <c r="AG53" s="1"/>
       <c r="AH53" s="1"/>
       <c r="AI53" s="1"/>
-      <c r="AJ53" s="56"/>
-      <c r="AK53" s="53"/>
-      <c r="AL53" s="68"/>
+      <c r="AJ53" s="52"/>
+      <c r="AK53" s="208"/>
+      <c r="AL53" s="138"/>
       <c r="AM53" s="1"/>
       <c r="AN53" s="1"/>
       <c r="AO53" s="1"/>
@@ -5205,39 +5205,39 @@
       <c r="A54" s="1">
         <v>1400</v>
       </c>
-      <c r="B54" s="156"/>
-      <c r="C54" s="189"/>
-      <c r="D54" s="168"/>
-      <c r="E54" s="174"/>
+      <c r="B54" s="142"/>
+      <c r="C54" s="211"/>
+      <c r="D54" s="160"/>
+      <c r="E54" s="163"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="191" t="s">
-        <v>164</v>
-      </c>
-      <c r="H54" s="178"/>
+      <c r="G54" s="213" t="s">
+        <v>161</v>
+      </c>
+      <c r="H54" s="167"/>
       <c r="I54" s="1"/>
-      <c r="J54" s="180"/>
-      <c r="K54" s="183"/>
+      <c r="J54" s="169"/>
+      <c r="K54" s="172"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
-      <c r="Q54" s="140"/>
+      <c r="Q54" s="133"/>
       <c r="R54" s="1"/>
-      <c r="S54" s="193" t="s">
+      <c r="S54" s="215" t="s">
+        <v>162</v>
+      </c>
+      <c r="T54" s="216"/>
+      <c r="U54" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="V54" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="W54" s="179" t="s">
         <v>165</v>
       </c>
-      <c r="T54" s="194"/>
-      <c r="U54" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="V54" s="196" t="s">
-        <v>167</v>
-      </c>
-      <c r="W54" s="198" t="s">
-        <v>168</v>
-      </c>
-      <c r="X54" s="199"/>
+      <c r="X54" s="180"/>
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
@@ -5249,9 +5249,9 @@
       <c r="AG54" s="1"/>
       <c r="AH54" s="1"/>
       <c r="AI54" s="1"/>
-      <c r="AJ54" s="56"/>
-      <c r="AK54" s="53"/>
-      <c r="AL54" s="69"/>
+      <c r="AJ54" s="52"/>
+      <c r="AK54" s="208"/>
+      <c r="AL54" s="139"/>
       <c r="AM54" s="1"/>
       <c r="AN54" s="1"/>
       <c r="AO54" s="1"/>
@@ -5263,39 +5263,39 @@
       <c r="A55" s="1">
         <v>1500</v>
       </c>
-      <c r="B55" s="185" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="189"/>
-      <c r="D55" s="168"/>
-      <c r="E55" s="174"/>
+      <c r="B55" s="191" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="211"/>
+      <c r="D55" s="160"/>
+      <c r="E55" s="163"/>
       <c r="F55" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="G55" s="192"/>
-      <c r="H55" s="200" t="s">
-        <v>170</v>
+        <v>166</v>
+      </c>
+      <c r="G55" s="214"/>
+      <c r="H55" s="194" t="s">
+        <v>167</v>
       </c>
       <c r="I55" s="1"/>
-      <c r="J55" s="180"/>
-      <c r="K55" s="183"/>
+      <c r="J55" s="169"/>
+      <c r="K55" s="172"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
-      <c r="P55" s="203" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q55" s="141"/>
-      <c r="R55" s="203" t="s">
-        <v>172</v>
-      </c>
-      <c r="S55" s="151"/>
-      <c r="T55" s="195"/>
+      <c r="P55" s="181" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q55" s="134"/>
+      <c r="R55" s="181" t="s">
+        <v>169</v>
+      </c>
+      <c r="S55" s="188"/>
+      <c r="T55" s="217"/>
       <c r="U55" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="V55" s="197"/>
+        <v>170</v>
+      </c>
+      <c r="V55" s="219"/>
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
       <c r="Y55" s="1"/>
@@ -5309,10 +5309,10 @@
       <c r="AG55" s="1"/>
       <c r="AH55" s="1"/>
       <c r="AI55" s="1"/>
-      <c r="AJ55" s="56"/>
-      <c r="AK55" s="53"/>
-      <c r="AL55" s="50" t="s">
-        <v>51</v>
+      <c r="AJ55" s="52"/>
+      <c r="AK55" s="208"/>
+      <c r="AL55" s="197" t="s">
+        <v>48</v>
       </c>
       <c r="AM55" s="1"/>
       <c r="AN55" s="1"/>
@@ -5325,44 +5325,44 @@
       <c r="A56" s="1">
         <v>1600</v>
       </c>
-      <c r="B56" s="186"/>
-      <c r="C56" s="189"/>
-      <c r="D56" s="169"/>
-      <c r="E56" s="174"/>
+      <c r="B56" s="192"/>
+      <c r="C56" s="211"/>
+      <c r="D56" s="161"/>
+      <c r="E56" s="163"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="218" t="s">
-        <v>174</v>
-      </c>
-      <c r="H56" s="201"/>
-      <c r="I56" s="221" t="s">
-        <v>175</v>
-      </c>
-      <c r="J56" s="181"/>
-      <c r="K56" s="183"/>
-      <c r="L56" s="223" t="s">
-        <v>176</v>
+      <c r="G56" s="199" t="s">
+        <v>171</v>
+      </c>
+      <c r="H56" s="195"/>
+      <c r="I56" s="202" t="s">
+        <v>172</v>
+      </c>
+      <c r="J56" s="170"/>
+      <c r="K56" s="172"/>
+      <c r="L56" s="204" t="s">
+        <v>173</v>
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
-      <c r="O56" s="203" t="s">
+      <c r="O56" s="181" t="s">
+        <v>174</v>
+      </c>
+      <c r="P56" s="182"/>
+      <c r="Q56" s="181" t="s">
+        <v>175</v>
+      </c>
+      <c r="R56" s="182"/>
+      <c r="S56" s="181" t="s">
+        <v>176</v>
+      </c>
+      <c r="T56" s="181" t="s">
         <v>177</v>
       </c>
-      <c r="P56" s="204"/>
-      <c r="Q56" s="203" t="s">
+      <c r="U56" s="181" t="s">
         <v>178</v>
       </c>
-      <c r="R56" s="204"/>
-      <c r="S56" s="203" t="s">
+      <c r="V56" s="174" t="s">
         <v>179</v>
-      </c>
-      <c r="T56" s="203" t="s">
-        <v>180</v>
-      </c>
-      <c r="U56" s="203" t="s">
-        <v>181</v>
-      </c>
-      <c r="V56" s="240" t="s">
-        <v>182</v>
       </c>
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
@@ -5377,9 +5377,9 @@
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
       <c r="AI56" s="1"/>
-      <c r="AJ56" s="56"/>
-      <c r="AK56" s="53"/>
-      <c r="AL56" s="51"/>
+      <c r="AJ56" s="52"/>
+      <c r="AK56" s="208"/>
+      <c r="AL56" s="198"/>
       <c r="AM56" s="1"/>
       <c r="AN56" s="1"/>
       <c r="AO56" s="1"/>
@@ -5391,31 +5391,31 @@
       <c r="A57" s="1">
         <v>1700</v>
       </c>
-      <c r="B57" s="187"/>
-      <c r="C57" s="190"/>
+      <c r="B57" s="193"/>
+      <c r="C57" s="212"/>
       <c r="D57" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="E57" s="175"/>
+        <v>180</v>
+      </c>
+      <c r="E57" s="164"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="219"/>
-      <c r="H57" s="201"/>
-      <c r="I57" s="222"/>
+      <c r="G57" s="200"/>
+      <c r="H57" s="195"/>
+      <c r="I57" s="203"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="183"/>
-      <c r="L57" s="224"/>
+      <c r="K57" s="172"/>
+      <c r="L57" s="205"/>
       <c r="M57" s="1"/>
-      <c r="N57" s="226" t="s">
-        <v>184</v>
-      </c>
-      <c r="O57" s="204"/>
-      <c r="P57" s="204"/>
-      <c r="Q57" s="204"/>
-      <c r="R57" s="204"/>
-      <c r="S57" s="204"/>
-      <c r="T57" s="204"/>
-      <c r="U57" s="204"/>
-      <c r="V57" s="241"/>
+      <c r="N57" s="177" t="s">
+        <v>181</v>
+      </c>
+      <c r="O57" s="182"/>
+      <c r="P57" s="182"/>
+      <c r="Q57" s="182"/>
+      <c r="R57" s="182"/>
+      <c r="S57" s="182"/>
+      <c r="T57" s="182"/>
+      <c r="U57" s="182"/>
+      <c r="V57" s="175"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
@@ -5429,10 +5429,10 @@
       <c r="AG57" s="1"/>
       <c r="AH57" s="1"/>
       <c r="AI57" s="1"/>
-      <c r="AJ57" s="56"/>
-      <c r="AK57" s="53"/>
+      <c r="AJ57" s="52"/>
+      <c r="AK57" s="208"/>
       <c r="AL57" s="31" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AM57" s="1"/>
       <c r="AN57" s="1"/>
@@ -5446,32 +5446,32 @@
         <v>1800</v>
       </c>
       <c r="B58" s="1"/>
-      <c r="C58" s="206" t="s">
-        <v>185</v>
-      </c>
-      <c r="D58" s="208" t="s">
-        <v>186</v>
-      </c>
-      <c r="E58" s="209"/>
+      <c r="C58" s="226" t="s">
+        <v>182</v>
+      </c>
+      <c r="D58" s="228" t="s">
+        <v>183</v>
+      </c>
+      <c r="E58" s="229"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="219"/>
-      <c r="H58" s="202"/>
+      <c r="G58" s="200"/>
+      <c r="H58" s="196"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="183"/>
-      <c r="L58" s="224"/>
-      <c r="M58" s="228" t="s">
-        <v>187</v>
-      </c>
-      <c r="N58" s="227"/>
-      <c r="O58" s="205"/>
-      <c r="P58" s="204"/>
-      <c r="Q58" s="204"/>
-      <c r="R58" s="204"/>
-      <c r="S58" s="204"/>
-      <c r="T58" s="204"/>
-      <c r="U58" s="204"/>
-      <c r="V58" s="241"/>
+      <c r="K58" s="172"/>
+      <c r="L58" s="205"/>
+      <c r="M58" s="234" t="s">
+        <v>184</v>
+      </c>
+      <c r="N58" s="178"/>
+      <c r="O58" s="183"/>
+      <c r="P58" s="182"/>
+      <c r="Q58" s="182"/>
+      <c r="R58" s="182"/>
+      <c r="S58" s="182"/>
+      <c r="T58" s="182"/>
+      <c r="U58" s="182"/>
+      <c r="V58" s="175"/>
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
       <c r="Y58" s="1"/>
@@ -5485,10 +5485,10 @@
       <c r="AG58" s="1"/>
       <c r="AH58" s="1"/>
       <c r="AI58" s="1"/>
-      <c r="AJ58" s="56"/>
-      <c r="AK58" s="54"/>
+      <c r="AJ58" s="52"/>
+      <c r="AK58" s="209"/>
       <c r="AL58" s="30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AM58" s="1"/>
       <c r="AN58" s="1"/>
@@ -5502,34 +5502,34 @@
         <v>1900</v>
       </c>
       <c r="B59" s="1"/>
-      <c r="C59" s="207"/>
-      <c r="D59" s="210"/>
-      <c r="E59" s="211"/>
+      <c r="C59" s="227"/>
+      <c r="D59" s="230"/>
+      <c r="E59" s="231"/>
       <c r="F59" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="G59" s="200"/>
+      <c r="H59" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="I59" s="1"/>
+      <c r="J59" s="237" t="s">
+        <v>187</v>
+      </c>
+      <c r="K59" s="172"/>
+      <c r="L59" s="205"/>
+      <c r="M59" s="235"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="240" t="s">
         <v>188</v>
       </c>
-      <c r="G59" s="219"/>
-      <c r="H59" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I59" s="1"/>
-      <c r="J59" s="231" t="s">
-        <v>190</v>
-      </c>
-      <c r="K59" s="183"/>
-      <c r="L59" s="224"/>
-      <c r="M59" s="229"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="234" t="s">
-        <v>191</v>
-      </c>
-      <c r="P59" s="205"/>
-      <c r="Q59" s="205"/>
-      <c r="R59" s="205"/>
-      <c r="S59" s="205"/>
-      <c r="T59" s="205"/>
-      <c r="U59" s="205"/>
-      <c r="V59" s="242"/>
+      <c r="P59" s="183"/>
+      <c r="Q59" s="183"/>
+      <c r="R59" s="183"/>
+      <c r="S59" s="183"/>
+      <c r="T59" s="183"/>
+      <c r="U59" s="183"/>
+      <c r="V59" s="176"/>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
       <c r="Y59" s="1"/>
@@ -5543,11 +5543,11 @@
       <c r="AG59" s="1"/>
       <c r="AH59" s="1"/>
       <c r="AI59" s="1"/>
-      <c r="AJ59" s="56"/>
-      <c r="AK59" s="237" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL59" s="238"/>
+      <c r="AJ59" s="52"/>
+      <c r="AK59" s="220" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL59" s="221"/>
       <c r="AM59" s="1"/>
       <c r="AN59" s="1"/>
       <c r="AO59" s="1"/>
@@ -5560,25 +5560,25 @@
         <v>2000</v>
       </c>
       <c r="B60" s="1"/>
-      <c r="C60" s="214" t="s">
-        <v>192</v>
-      </c>
-      <c r="D60" s="210"/>
-      <c r="E60" s="211"/>
+      <c r="C60" s="222" t="s">
+        <v>189</v>
+      </c>
+      <c r="D60" s="230"/>
+      <c r="E60" s="231"/>
       <c r="F60" s="1"/>
-      <c r="G60" s="219"/>
-      <c r="H60" s="176" t="s">
-        <v>193</v>
-      </c>
-      <c r="I60" s="216" t="s">
-        <v>194</v>
-      </c>
-      <c r="J60" s="232"/>
-      <c r="K60" s="183"/>
-      <c r="L60" s="224"/>
-      <c r="M60" s="229"/>
+      <c r="G60" s="200"/>
+      <c r="H60" s="165" t="s">
+        <v>190</v>
+      </c>
+      <c r="I60" s="224" t="s">
+        <v>191</v>
+      </c>
+      <c r="J60" s="238"/>
+      <c r="K60" s="172"/>
+      <c r="L60" s="205"/>
+      <c r="M60" s="235"/>
       <c r="N60" s="1"/>
-      <c r="O60" s="235"/>
+      <c r="O60" s="241"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -5598,11 +5598,11 @@
       <c r="AG60" s="1"/>
       <c r="AH60" s="1"/>
       <c r="AI60" s="1"/>
-      <c r="AJ60" s="56"/>
-      <c r="AK60" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL60" s="50"/>
+      <c r="AJ60" s="52"/>
+      <c r="AK60" s="207" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL60" s="197"/>
       <c r="AM60" s="1"/>
       <c r="AN60" s="1"/>
       <c r="AO60" s="1"/>
@@ -5615,19 +5615,19 @@
         <v>2100</v>
       </c>
       <c r="B61" s="1"/>
-      <c r="C61" s="215"/>
-      <c r="D61" s="212"/>
-      <c r="E61" s="213"/>
+      <c r="C61" s="223"/>
+      <c r="D61" s="232"/>
+      <c r="E61" s="233"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="220"/>
-      <c r="H61" s="178"/>
-      <c r="I61" s="217"/>
-      <c r="J61" s="233"/>
-      <c r="K61" s="184"/>
-      <c r="L61" s="225"/>
-      <c r="M61" s="230"/>
+      <c r="G61" s="201"/>
+      <c r="H61" s="167"/>
+      <c r="I61" s="225"/>
+      <c r="J61" s="239"/>
+      <c r="K61" s="173"/>
+      <c r="L61" s="206"/>
+      <c r="M61" s="236"/>
       <c r="N61" s="1"/>
-      <c r="O61" s="236"/>
+      <c r="O61" s="242"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -5647,9 +5647,9 @@
       <c r="AG61" s="1"/>
       <c r="AH61" s="1"/>
       <c r="AI61" s="1"/>
-      <c r="AJ61" s="57"/>
-      <c r="AK61" s="54"/>
-      <c r="AL61" s="51"/>
+      <c r="AJ61" s="53"/>
+      <c r="AK61" s="209"/>
+      <c r="AL61" s="198"/>
       <c r="AM61" s="1"/>
       <c r="AN61" s="1"/>
       <c r="AO61" s="1"/>
@@ -5659,20 +5659,10 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="C58:C59"/>
     <mergeCell ref="D58:E61"/>
     <mergeCell ref="M58:M61"/>
     <mergeCell ref="J59:J61"/>
     <mergeCell ref="O59:O61"/>
-    <mergeCell ref="AK59:AL59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="AK60:AL61"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="H55:H58"/>
-    <mergeCell ref="P55:P59"/>
-    <mergeCell ref="R55:R59"/>
     <mergeCell ref="AL55:AL56"/>
     <mergeCell ref="G56:G61"/>
     <mergeCell ref="I56:I57"/>
@@ -5681,33 +5671,37 @@
     <mergeCell ref="Q56:Q59"/>
     <mergeCell ref="AK51:AK58"/>
     <mergeCell ref="AJ52:AJ61"/>
-    <mergeCell ref="C53:C57"/>
     <mergeCell ref="G54:G55"/>
     <mergeCell ref="S54:T55"/>
     <mergeCell ref="V54:V55"/>
+    <mergeCell ref="AK59:AL59"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="AK60:AL61"/>
+    <mergeCell ref="V56:V59"/>
+    <mergeCell ref="N57:N58"/>
     <mergeCell ref="W54:X54"/>
     <mergeCell ref="S56:S59"/>
     <mergeCell ref="T56:T59"/>
     <mergeCell ref="U56:U59"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="U49:U50"/>
-    <mergeCell ref="V49:V50"/>
-    <mergeCell ref="E50:E57"/>
-    <mergeCell ref="H50:H54"/>
-    <mergeCell ref="J51:J56"/>
-    <mergeCell ref="K51:K61"/>
-    <mergeCell ref="V56:V59"/>
-    <mergeCell ref="N57:N58"/>
-    <mergeCell ref="T45:T46"/>
-    <mergeCell ref="AL45:AL54"/>
+    <mergeCell ref="P55:P59"/>
+    <mergeCell ref="R55:R59"/>
     <mergeCell ref="B46:B54"/>
     <mergeCell ref="I46:I48"/>
     <mergeCell ref="L46:L47"/>
     <mergeCell ref="N46:N47"/>
     <mergeCell ref="K47:K49"/>
-    <mergeCell ref="R48:R51"/>
-    <mergeCell ref="S48:W48"/>
     <mergeCell ref="D49:D56"/>
+    <mergeCell ref="E50:E57"/>
+    <mergeCell ref="H50:H54"/>
+    <mergeCell ref="J51:J56"/>
+    <mergeCell ref="K51:K61"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="H55:H58"/>
+    <mergeCell ref="C53:C57"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C58:C59"/>
     <mergeCell ref="AL41:AN44"/>
     <mergeCell ref="E42:E44"/>
     <mergeCell ref="P42:P44"/>
@@ -5718,6 +5712,12 @@
     <mergeCell ref="Q45:Q55"/>
     <mergeCell ref="R45:R46"/>
     <mergeCell ref="S45:S46"/>
+    <mergeCell ref="T45:T46"/>
+    <mergeCell ref="AL45:AL54"/>
+    <mergeCell ref="R48:R51"/>
+    <mergeCell ref="S48:W48"/>
+    <mergeCell ref="U49:U50"/>
+    <mergeCell ref="V49:V50"/>
     <mergeCell ref="W36:X36"/>
     <mergeCell ref="Q37:R37"/>
     <mergeCell ref="S38:S40"/>
@@ -5738,12 +5738,6 @@
     <mergeCell ref="M41:M45"/>
     <mergeCell ref="N41:N44"/>
     <mergeCell ref="S41:S44"/>
-    <mergeCell ref="S26:S30"/>
-    <mergeCell ref="T26:T28"/>
-    <mergeCell ref="B29:B35"/>
-    <mergeCell ref="R29:R33"/>
-    <mergeCell ref="S31:S33"/>
-    <mergeCell ref="M33:M35"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="U2:U17"/>
     <mergeCell ref="B7:B28"/>
@@ -5754,6 +5748,12 @@
     <mergeCell ref="U21:U22"/>
     <mergeCell ref="R24:R28"/>
     <mergeCell ref="U24:U25"/>
+    <mergeCell ref="S26:S30"/>
+    <mergeCell ref="T26:T28"/>
+    <mergeCell ref="B29:B35"/>
+    <mergeCell ref="R29:R33"/>
+    <mergeCell ref="S31:S33"/>
+    <mergeCell ref="M33:M35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
WEBSITE ONLINE!!, Balkans Reworked
I put Greece and Thrace together into a region called the eastern mediterannean, and I added the adriatic coast. I also updated the SVG with those borders and put the Germania border on. I then updated the data in the excel files for these new regions and added a couple powers that were under represented, namely the franks and east francia. Also, this iteration put my website online so, pretty big stuff.
</commit_message>
<xml_diff>
--- a/BigOlTimeline_Chart.xlsx
+++ b/BigOlTimeline_Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\Personal\BigOlTimeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB123BB1-487E-4A61-A63F-927EBD5A3699}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6803CD97-38FF-4ED7-A28C-9518CD247AD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12510" yWindow="4725" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="198">
   <si>
     <t>Ireland</t>
   </si>
@@ -60,12 +60,6 @@
     <t>North Africa</t>
   </si>
   <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Thrace</t>
-  </si>
-  <si>
     <t>Constaninople</t>
   </si>
   <si>
@@ -288,9 +282,6 @@
     <t> Republic: 509-27BC</t>
   </si>
   <si>
-    <t>513-478</t>
-  </si>
-  <si>
     <t>546-334</t>
   </si>
   <si>
@@ -306,12 +297,6 @@
     <t>Achaemenid Persia: 550-328</t>
   </si>
   <si>
-    <t>337-301</t>
-  </si>
-  <si>
-    <t>Macedonia: 342-301</t>
-  </si>
-  <si>
     <t>333-301</t>
   </si>
   <si>
@@ -345,9 +330,6 @@
     <t>Numidia: 202-107</t>
   </si>
   <si>
-    <t>147BC-395AD</t>
-  </si>
-  <si>
     <t>197-84</t>
   </si>
   <si>
@@ -378,21 +360,12 @@
     <t>59-410</t>
   </si>
   <si>
-    <t>47-395</t>
-  </si>
-  <si>
     <t>227-642</t>
   </si>
   <si>
     <t>Sassanid: 220-650: Rashidun: 651-661</t>
   </si>
   <si>
-    <t>295-1204</t>
-  </si>
-  <si>
-    <t>395-1190</t>
-  </si>
-  <si>
     <t>Byzantine Empire: 395-1453</t>
   </si>
   <si>
@@ -465,9 +438,6 @@
     <t>Poland: 966-1386</t>
   </si>
   <si>
-    <t>German Franks:930-962</t>
-  </si>
-  <si>
     <t>Samanid: 901-998</t>
   </si>
   <si>
@@ -555,9 +525,6 @@
     <t>Spain: 1480-Present</t>
   </si>
   <si>
-    <t>1461-1829</t>
-  </si>
-  <si>
     <t>Ottoman Empire: 1454-1922</t>
   </si>
   <si>
@@ -597,9 +564,6 @@
     <t>Germany: 1872-Present</t>
   </si>
   <si>
-    <t>Greece: 1830-Present</t>
-  </si>
-  <si>
     <t>Ireland: 1923-Present</t>
   </si>
   <si>
@@ -616,6 +580,51 @@
   </si>
   <si>
     <t>Italia</t>
+  </si>
+  <si>
+    <t>Adriatic Coast</t>
+  </si>
+  <si>
+    <t>Eastern Mediterranean</t>
+  </si>
+  <si>
+    <t>168BC-395AD</t>
+  </si>
+  <si>
+    <t>Macedonia: 337-301</t>
+  </si>
+  <si>
+    <t>395-803</t>
+  </si>
+  <si>
+    <t>Franks: 803-845</t>
+  </si>
+  <si>
+    <t>German Franks:900-962</t>
+  </si>
+  <si>
+    <t>783-843; East Francia: 843-900</t>
+  </si>
+  <si>
+    <t>1464-1879</t>
+  </si>
+  <si>
+    <t>Austria-Hungary: 1879-1918; Yugoslavia: 1919-1991</t>
+  </si>
+  <si>
+    <t>Hungary: 1138-1284</t>
+  </si>
+  <si>
+    <t>29BC-395</t>
+  </si>
+  <si>
+    <t>395-917</t>
+  </si>
+  <si>
+    <t>Bulgaria: 917-972</t>
+  </si>
+  <si>
+    <t>1018-1204</t>
   </si>
 </sst>
 </file>
@@ -631,7 +640,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="53">
+  <fills count="52">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -935,12 +944,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF892B2A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0663A9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1312,7 +1315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1413,9 +1416,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1428,9 +1428,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1438,9 +1435,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1464,6 +1458,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1471,6 +1549,387 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1506,9 +1965,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1563,481 +2019,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="48" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="48" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="48" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="49" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="49" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="49" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="52" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="52" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="52" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2336,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7CFCAE-E1AA-4E44-87FB-807FA0F08CCC}">
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56:I57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2353,7 +2350,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2374,111 +2371,111 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3800</v>
       </c>
-      <c r="B2" s="51" t="s">
-        <v>38</v>
+      <c r="B2" s="76" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2498,8 +2495,8 @@
       <c r="R2" s="1"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
-      <c r="U2" s="54" t="s">
-        <v>57</v>
+      <c r="U2" s="206" t="s">
+        <v>55</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
@@ -2529,7 +2526,7 @@
       <c r="A3" s="1">
         <v>3700</v>
       </c>
-      <c r="B3" s="52"/>
+      <c r="B3" s="77"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2548,7 +2545,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="55"/>
+      <c r="U3" s="207"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -2577,7 +2574,7 @@
       <c r="A4" s="1">
         <v>3600</v>
       </c>
-      <c r="B4" s="52"/>
+      <c r="B4" s="77"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2596,7 +2593,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="55"/>
+      <c r="U4" s="207"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -2625,7 +2622,7 @@
       <c r="A5" s="1">
         <v>3500</v>
       </c>
-      <c r="B5" s="52"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2644,7 +2641,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
-      <c r="U5" s="55"/>
+      <c r="U5" s="207"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
@@ -2673,7 +2670,7 @@
       <c r="A6" s="1">
         <v>3400</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2692,7 +2689,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-      <c r="U6" s="55"/>
+      <c r="U6" s="207"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -2721,8 +2718,8 @@
       <c r="A7" s="1">
         <v>3300</v>
       </c>
-      <c r="B7" s="57" t="s">
-        <v>58</v>
+      <c r="B7" s="209" t="s">
+        <v>56</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2742,7 +2739,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="55"/>
+      <c r="U7" s="207"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
@@ -2771,7 +2768,7 @@
       <c r="A8" s="1">
         <v>3200</v>
       </c>
-      <c r="B8" s="58"/>
+      <c r="B8" s="210"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2790,7 +2787,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
-      <c r="U8" s="55"/>
+      <c r="U8" s="207"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -2819,7 +2816,7 @@
       <c r="A9" s="1">
         <v>3100</v>
       </c>
-      <c r="B9" s="58"/>
+      <c r="B9" s="210"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2836,11 +2833,11 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="60" t="s">
-        <v>59</v>
+      <c r="S9" s="212" t="s">
+        <v>57</v>
       </c>
       <c r="T9" s="3"/>
-      <c r="U9" s="55"/>
+      <c r="U9" s="207"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
@@ -2869,7 +2866,7 @@
       <c r="A10" s="1">
         <v>3000</v>
       </c>
-      <c r="B10" s="58"/>
+      <c r="B10" s="210"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2886,9 +2883,9 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="61"/>
+      <c r="S10" s="213"/>
       <c r="T10" s="3"/>
-      <c r="U10" s="55"/>
+      <c r="U10" s="207"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
@@ -2917,7 +2914,7 @@
       <c r="A11" s="1">
         <v>2900</v>
       </c>
-      <c r="B11" s="58"/>
+      <c r="B11" s="210"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2934,9 +2931,9 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="61"/>
+      <c r="S11" s="213"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="55"/>
+      <c r="U11" s="207"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
@@ -2965,7 +2962,7 @@
       <c r="A12" s="1">
         <v>2800</v>
       </c>
-      <c r="B12" s="58"/>
+      <c r="B12" s="210"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2982,9 +2979,9 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="61"/>
+      <c r="S12" s="213"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="55"/>
+      <c r="U12" s="207"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -3013,7 +3010,7 @@
       <c r="A13" s="1">
         <v>2700</v>
       </c>
-      <c r="B13" s="58"/>
+      <c r="B13" s="210"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -3030,9 +3027,9 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="61"/>
+      <c r="S13" s="213"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="55"/>
+      <c r="U13" s="207"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -3061,7 +3058,7 @@
       <c r="A14" s="1">
         <v>2600</v>
       </c>
-      <c r="B14" s="58"/>
+      <c r="B14" s="210"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3078,9 +3075,9 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
-      <c r="S14" s="61"/>
+      <c r="S14" s="213"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="55"/>
+      <c r="U14" s="207"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -3109,7 +3106,7 @@
       <c r="A15" s="1">
         <v>2500</v>
       </c>
-      <c r="B15" s="58"/>
+      <c r="B15" s="210"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -3126,11 +3123,11 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="61" t="s">
-        <v>60</v>
+      <c r="S15" s="213" t="s">
+        <v>58</v>
       </c>
       <c r="T15" s="3"/>
-      <c r="U15" s="55"/>
+      <c r="U15" s="207"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
@@ -3159,7 +3156,7 @@
       <c r="A16" s="1">
         <v>2400</v>
       </c>
-      <c r="B16" s="58"/>
+      <c r="B16" s="210"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -3176,9 +3173,9 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="61"/>
+      <c r="S16" s="213"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="55"/>
+      <c r="U16" s="207"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
@@ -3207,7 +3204,7 @@
       <c r="A17" s="1">
         <v>2300</v>
       </c>
-      <c r="B17" s="58"/>
+      <c r="B17" s="210"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -3224,9 +3221,9 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="61"/>
+      <c r="S17" s="213"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="56"/>
+      <c r="U17" s="208"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -3255,7 +3252,7 @@
       <c r="A18" s="1">
         <v>2200</v>
       </c>
-      <c r="B18" s="58"/>
+      <c r="B18" s="210"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3272,10 +3269,10 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="61"/>
+      <c r="S18" s="213"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="62" t="s">
-        <v>61</v>
+      <c r="U18" s="214" t="s">
+        <v>59</v>
       </c>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
@@ -3305,7 +3302,7 @@
       <c r="A19" s="1">
         <v>2100</v>
       </c>
-      <c r="B19" s="58"/>
+      <c r="B19" s="210"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3322,11 +3319,11 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-      <c r="S19" s="41" t="s">
-        <v>62</v>
+      <c r="S19" s="39" t="s">
+        <v>60</v>
       </c>
       <c r="T19" s="3"/>
-      <c r="U19" s="63"/>
+      <c r="U19" s="215"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
@@ -3355,7 +3352,7 @@
       <c r="A20" s="1">
         <v>2000</v>
       </c>
-      <c r="B20" s="58"/>
+      <c r="B20" s="210"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -3372,8 +3369,8 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-      <c r="S20" s="64" t="s">
-        <v>63</v>
+      <c r="S20" s="216" t="s">
+        <v>61</v>
       </c>
       <c r="T20" s="28"/>
       <c r="U20" s="1"/>
@@ -3405,7 +3402,7 @@
       <c r="A21" s="1">
         <v>1900</v>
       </c>
-      <c r="B21" s="58"/>
+      <c r="B21" s="210"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -3422,10 +3419,10 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="64"/>
+      <c r="S21" s="216"/>
       <c r="T21" s="28"/>
-      <c r="U21" s="65" t="s">
-        <v>64</v>
+      <c r="U21" s="158" t="s">
+        <v>62</v>
       </c>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
@@ -3455,7 +3452,7 @@
       <c r="A22" s="1">
         <v>1800</v>
       </c>
-      <c r="B22" s="58"/>
+      <c r="B22" s="210"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -3472,11 +3469,11 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="64"/>
+      <c r="S22" s="216"/>
       <c r="T22" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="U22" s="66"/>
+        <v>63</v>
+      </c>
+      <c r="U22" s="217"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
@@ -3505,7 +3502,7 @@
       <c r="A23" s="1">
         <v>1700</v>
       </c>
-      <c r="B23" s="58"/>
+      <c r="B23" s="210"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -3522,7 +3519,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-      <c r="S23" s="64"/>
+      <c r="S23" s="216"/>
       <c r="T23" s="28"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
@@ -3553,7 +3550,7 @@
       <c r="A24" s="1">
         <v>1600</v>
       </c>
-      <c r="B24" s="58"/>
+      <c r="B24" s="210"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -3569,13 +3566,13 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="S24" s="64"/>
+      <c r="R24" s="218" t="s">
+        <v>64</v>
+      </c>
+      <c r="S24" s="216"/>
       <c r="T24" s="28"/>
-      <c r="U24" s="70" t="s">
-        <v>67</v>
+      <c r="U24" s="221" t="s">
+        <v>65</v>
       </c>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
@@ -3605,7 +3602,7 @@
       <c r="A25" s="1">
         <v>1500</v>
       </c>
-      <c r="B25" s="58"/>
+      <c r="B25" s="210"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -3621,12 +3618,12 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="68"/>
-      <c r="S25" s="41" t="s">
-        <v>68</v>
+      <c r="R25" s="219"/>
+      <c r="S25" s="39" t="s">
+        <v>66</v>
       </c>
       <c r="T25" s="3"/>
-      <c r="U25" s="71"/>
+      <c r="U25" s="222"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -3655,7 +3652,7 @@
       <c r="A26" s="1">
         <v>1400</v>
       </c>
-      <c r="B26" s="58"/>
+      <c r="B26" s="210"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -3671,12 +3668,12 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="68"/>
-      <c r="S26" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="T26" s="72" t="s">
-        <v>70</v>
+      <c r="R26" s="219"/>
+      <c r="S26" s="216" t="s">
+        <v>67</v>
+      </c>
+      <c r="T26" s="223" t="s">
+        <v>68</v>
       </c>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
@@ -3707,7 +3704,7 @@
       <c r="A27" s="1">
         <v>1300</v>
       </c>
-      <c r="B27" s="58"/>
+      <c r="B27" s="210"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -3723,9 +3720,9 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="68"/>
-      <c r="S27" s="64"/>
-      <c r="T27" s="73"/>
+      <c r="R27" s="219"/>
+      <c r="S27" s="216"/>
+      <c r="T27" s="224"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
@@ -3755,7 +3752,7 @@
       <c r="A28" s="1">
         <v>1200</v>
       </c>
-      <c r="B28" s="59"/>
+      <c r="B28" s="211"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -3771,9 +3768,9 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="69"/>
-      <c r="S28" s="64"/>
-      <c r="T28" s="74"/>
+      <c r="R28" s="220"/>
+      <c r="S28" s="216"/>
+      <c r="T28" s="225"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
@@ -3803,8 +3800,8 @@
       <c r="A29" s="1">
         <v>1100</v>
       </c>
-      <c r="B29" s="75" t="s">
-        <v>53</v>
+      <c r="B29" s="226" t="s">
+        <v>51</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -3821,10 +3818,10 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="S29" s="64"/>
+      <c r="R29" s="229" t="s">
+        <v>69</v>
+      </c>
+      <c r="S29" s="216"/>
       <c r="T29" s="28"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
@@ -3855,7 +3852,7 @@
       <c r="A30" s="1">
         <v>1000</v>
       </c>
-      <c r="B30" s="76"/>
+      <c r="B30" s="227"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -3871,8 +3868,8 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="79"/>
-      <c r="S30" s="64"/>
+      <c r="R30" s="230"/>
+      <c r="S30" s="216"/>
       <c r="T30" s="28"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
@@ -3903,7 +3900,7 @@
       <c r="A31" s="1">
         <v>900</v>
       </c>
-      <c r="B31" s="76"/>
+      <c r="B31" s="227"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -3919,12 +3916,12 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
-      <c r="R31" s="79"/>
-      <c r="S31" s="81" t="s">
-        <v>72</v>
+      <c r="R31" s="230"/>
+      <c r="S31" s="232" t="s">
+        <v>70</v>
       </c>
       <c r="T31" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
@@ -3955,7 +3952,7 @@
       <c r="A32" s="1">
         <v>800</v>
       </c>
-      <c r="B32" s="76"/>
+      <c r="B32" s="227"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -3971,8 +3968,8 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="79"/>
-      <c r="S32" s="81"/>
+      <c r="R32" s="230"/>
+      <c r="S32" s="232"/>
       <c r="T32" s="28"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
@@ -4003,7 +4000,7 @@
       <c r="A33" s="1">
         <v>700</v>
       </c>
-      <c r="B33" s="76"/>
+      <c r="B33" s="227"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -4014,18 +4011,18 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="82" t="s">
-        <v>74</v>
+      <c r="M33" s="233" t="s">
+        <v>72</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="80"/>
-      <c r="S33" s="81"/>
+      <c r="R33" s="231"/>
+      <c r="S33" s="232"/>
       <c r="T33" s="33"/>
-      <c r="U33" s="84" t="s">
-        <v>75</v>
+      <c r="U33" s="193" t="s">
+        <v>73</v>
       </c>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
@@ -4055,7 +4052,7 @@
       <c r="A34" s="1">
         <v>600</v>
       </c>
-      <c r="B34" s="76"/>
+      <c r="B34" s="227"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -4066,23 +4063,23 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-      <c r="M34" s="83"/>
-      <c r="N34" s="86" t="s">
-        <v>76</v>
+      <c r="M34" s="234"/>
+      <c r="N34" s="195" t="s">
+        <v>74</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
-      <c r="Q34" s="89" t="s">
+      <c r="Q34" s="198" t="s">
+        <v>75</v>
+      </c>
+      <c r="R34" s="199"/>
+      <c r="S34" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="T34" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="R34" s="90"/>
-      <c r="S34" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="T34" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="U34" s="85"/>
+      <c r="U34" s="194"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
@@ -4111,7 +4108,7 @@
       <c r="A35" s="1">
         <v>500</v>
       </c>
-      <c r="B35" s="77"/>
+      <c r="B35" s="228"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -4122,24 +4119,24 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="83"/>
-      <c r="N35" s="87"/>
+      <c r="M35" s="234"/>
+      <c r="N35" s="196"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-      <c r="Q35" s="91"/>
-      <c r="R35" s="92"/>
+      <c r="Q35" s="200"/>
+      <c r="R35" s="201"/>
       <c r="S35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="T35" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="U35" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="T35" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="U35" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="V35" s="1"/>
       <c r="W35" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
@@ -4167,8 +4164,8 @@
       <c r="A36" s="1">
         <v>400</v>
       </c>
-      <c r="B36" s="93" t="s">
-        <v>54</v>
+      <c r="B36" s="202" t="s">
+        <v>52</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -4180,32 +4177,30 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="96" t="s">
+      <c r="M36" s="151" t="s">
+        <v>82</v>
+      </c>
+      <c r="N36" s="196"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="239" t="s">
+        <v>83</v>
+      </c>
+      <c r="R36" s="240"/>
+      <c r="S36" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="N36" s="87"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="43" t="s">
+      <c r="T36" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="Q36" s="98" t="s">
+      <c r="U36" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R36" s="98"/>
-      <c r="S36" s="42" t="s">
+      <c r="V36" s="1"/>
+      <c r="W36" s="178" t="s">
         <v>87</v>
       </c>
-      <c r="T36" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="U36" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="V36" s="1"/>
-      <c r="W36" s="103" t="s">
-        <v>90</v>
-      </c>
-      <c r="X36" s="104"/>
+      <c r="X36" s="179"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
@@ -4231,7 +4226,7 @@
       <c r="A37" s="1">
         <v>300</v>
       </c>
-      <c r="B37" s="94"/>
+      <c r="B37" s="203"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -4242,33 +4237,31 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
-      <c r="M37" s="96"/>
-      <c r="N37" s="87"/>
-      <c r="O37" s="9" t="s">
+      <c r="M37" s="151"/>
+      <c r="N37" s="196"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q37" s="180" t="s">
+        <v>88</v>
+      </c>
+      <c r="R37" s="181"/>
+      <c r="S37" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="T37" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="U37" s="38" t="s">
         <v>91</v>
-      </c>
-      <c r="P37" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q37" s="105" t="s">
-        <v>93</v>
-      </c>
-      <c r="R37" s="106"/>
-      <c r="S37" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="T37" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="U37" s="40" t="s">
-        <v>96</v>
       </c>
       <c r="V37" s="1"/>
       <c r="W37" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="X37" s="40" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="X37" s="38" t="s">
+        <v>93</v>
       </c>
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
@@ -4295,7 +4288,7 @@
       <c r="A38" s="1">
         <v>200</v>
       </c>
-      <c r="B38" s="94"/>
+      <c r="B38" s="203"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -4306,20 +4299,20 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="96"/>
-      <c r="N38" s="88"/>
+      <c r="M38" s="151"/>
+      <c r="N38" s="197"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="S38" s="107" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="S38" s="182" t="s">
+        <v>95</v>
       </c>
       <c r="T38" s="1"/>
-      <c r="U38" s="110" t="s">
-        <v>101</v>
+      <c r="U38" s="185" t="s">
+        <v>96</v>
       </c>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
@@ -4349,7 +4342,7 @@
       <c r="A39" s="1">
         <v>100</v>
       </c>
-      <c r="B39" s="94"/>
+      <c r="B39" s="203"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -4358,27 +4351,27 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="99" t="s">
-        <v>102</v>
-      </c>
-      <c r="M39" s="97"/>
-      <c r="N39" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="O39" s="99" t="s">
-        <v>104</v>
+      <c r="K39" s="35"/>
+      <c r="L39" s="187" t="s">
+        <v>97</v>
+      </c>
+      <c r="M39" s="191"/>
+      <c r="N39" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="O39" s="187" t="s">
+        <v>185</v>
       </c>
       <c r="P39" s="28"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="108"/>
+      <c r="S39" s="183"/>
       <c r="T39" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="U39" s="111"/>
-      <c r="W39" s="112" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="U39" s="186"/>
+      <c r="W39" s="188" t="s">
+        <v>100</v>
       </c>
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
@@ -4406,7 +4399,7 @@
       <c r="A40" s="1">
         <v>0</v>
       </c>
-      <c r="B40" s="94"/>
+      <c r="B40" s="203"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -4414,27 +4407,29 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="99" t="s">
-        <v>107</v>
-      </c>
-      <c r="L40" s="100"/>
-      <c r="M40" s="97"/>
-      <c r="N40" s="38"/>
-      <c r="O40" s="100"/>
-      <c r="P40" s="34"/>
-      <c r="Q40" s="99" t="s">
-        <v>108</v>
-      </c>
-      <c r="R40" s="99"/>
-      <c r="S40" s="109"/>
-      <c r="T40" s="115" t="s">
-        <v>108</v>
-      </c>
-      <c r="U40" s="112" t="s">
-        <v>109</v>
-      </c>
-      <c r="W40" s="113"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="187" t="s">
+        <v>101</v>
+      </c>
+      <c r="L40" s="153"/>
+      <c r="M40" s="191"/>
+      <c r="N40" s="37"/>
+      <c r="O40" s="153"/>
+      <c r="P40" s="187" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q40" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="R40" s="187"/>
+      <c r="S40" s="184"/>
+      <c r="T40" s="150" t="s">
+        <v>102</v>
+      </c>
+      <c r="U40" s="188" t="s">
+        <v>103</v>
+      </c>
+      <c r="W40" s="189"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
@@ -4461,7 +4456,7 @@
       <c r="A41" s="1">
         <v>100</v>
       </c>
-      <c r="B41" s="94"/>
+      <c r="B41" s="203"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -4470,26 +4465,26 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="K41" s="100"/>
-      <c r="L41" s="100"/>
-      <c r="M41" s="100" t="s">
-        <v>111</v>
-      </c>
-      <c r="N41" s="99" t="s">
-        <v>112</v>
-      </c>
-      <c r="O41" s="100"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="100"/>
-      <c r="R41" s="100"/>
-      <c r="S41" s="99" t="s">
-        <v>113</v>
-      </c>
-      <c r="T41" s="97"/>
-      <c r="U41" s="113"/>
-      <c r="W41" s="113"/>
+        <v>104</v>
+      </c>
+      <c r="K41" s="153"/>
+      <c r="L41" s="153"/>
+      <c r="M41" s="153" t="s">
+        <v>105</v>
+      </c>
+      <c r="N41" s="187" t="s">
+        <v>106</v>
+      </c>
+      <c r="O41" s="153"/>
+      <c r="P41" s="153"/>
+      <c r="Q41" s="153"/>
+      <c r="R41" s="153"/>
+      <c r="S41" s="187" t="s">
+        <v>107</v>
+      </c>
+      <c r="T41" s="191"/>
+      <c r="U41" s="189"/>
+      <c r="W41" s="189"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
@@ -4504,13 +4499,13 @@
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL41" s="117" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM41" s="118"/>
-      <c r="AN41" s="119"/>
+        <v>37</v>
+      </c>
+      <c r="AL41" s="141" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM41" s="142"/>
+      <c r="AN41" s="143"/>
       <c r="AO41" s="1"/>
       <c r="AP41" s="1"/>
       <c r="AQ41" s="1"/>
@@ -4520,31 +4515,29 @@
       <c r="A42" s="1">
         <v>200</v>
       </c>
-      <c r="B42" s="94"/>
+      <c r="B42" s="203"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="115" t="s">
-        <v>114</v>
+      <c r="E42" s="150" t="s">
+        <v>108</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="100"/>
-      <c r="L42" s="100"/>
-      <c r="M42" s="100"/>
-      <c r="N42" s="100"/>
-      <c r="O42" s="100"/>
-      <c r="P42" s="100" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q42" s="100"/>
-      <c r="R42" s="100"/>
-      <c r="S42" s="100"/>
-      <c r="T42" s="97"/>
-      <c r="U42" s="114"/>
-      <c r="W42" s="114"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="153"/>
+      <c r="L42" s="153"/>
+      <c r="M42" s="153"/>
+      <c r="N42" s="153"/>
+      <c r="O42" s="153"/>
+      <c r="P42" s="153"/>
+      <c r="Q42" s="153"/>
+      <c r="R42" s="153"/>
+      <c r="S42" s="153"/>
+      <c r="T42" s="191"/>
+      <c r="U42" s="190"/>
+      <c r="W42" s="190"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
@@ -4559,11 +4552,11 @@
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL42" s="120"/>
-      <c r="AM42" s="121"/>
-      <c r="AN42" s="122"/>
+        <v>39</v>
+      </c>
+      <c r="AL42" s="144"/>
+      <c r="AM42" s="145"/>
+      <c r="AN42" s="146"/>
       <c r="AO42" s="1"/>
       <c r="AP42" s="1"/>
       <c r="AQ42" s="1"/>
@@ -4573,31 +4566,31 @@
       <c r="A43" s="1">
         <v>300</v>
       </c>
-      <c r="B43" s="94"/>
+      <c r="B43" s="203"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="96"/>
+      <c r="E43" s="151"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="7"/>
-      <c r="K43" s="100"/>
-      <c r="L43" s="100"/>
-      <c r="M43" s="100"/>
-      <c r="N43" s="100"/>
-      <c r="O43" s="100"/>
-      <c r="P43" s="100"/>
-      <c r="Q43" s="100"/>
-      <c r="R43" s="100"/>
-      <c r="S43" s="100"/>
-      <c r="T43" s="97"/>
-      <c r="U43" s="127" t="s">
-        <v>116</v>
-      </c>
-      <c r="V43" s="50"/>
-      <c r="W43" s="65" t="s">
-        <v>117</v>
+      <c r="K43" s="153"/>
+      <c r="L43" s="153"/>
+      <c r="M43" s="153"/>
+      <c r="N43" s="153"/>
+      <c r="O43" s="153"/>
+      <c r="P43" s="153"/>
+      <c r="Q43" s="153"/>
+      <c r="R43" s="153"/>
+      <c r="S43" s="153"/>
+      <c r="T43" s="191"/>
+      <c r="U43" s="155" t="s">
+        <v>109</v>
+      </c>
+      <c r="V43" s="47"/>
+      <c r="W43" s="158" t="s">
+        <v>110</v>
       </c>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
@@ -4613,11 +4606,11 @@
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL43" s="120"/>
-      <c r="AM43" s="121"/>
-      <c r="AN43" s="122"/>
+        <v>40</v>
+      </c>
+      <c r="AL43" s="144"/>
+      <c r="AM43" s="145"/>
+      <c r="AN43" s="146"/>
       <c r="AO43" s="1"/>
       <c r="AP43" s="1"/>
       <c r="AQ43" s="1"/>
@@ -4627,28 +4620,28 @@
       <c r="A44" s="1">
         <v>400</v>
       </c>
-      <c r="B44" s="94"/>
+      <c r="B44" s="203"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="126"/>
+      <c r="E44" s="152"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="7"/>
-      <c r="K44" s="100"/>
-      <c r="L44" s="100"/>
-      <c r="M44" s="100"/>
-      <c r="N44" s="101"/>
-      <c r="O44" s="101"/>
-      <c r="P44" s="101"/>
-      <c r="Q44" s="101"/>
-      <c r="R44" s="101"/>
-      <c r="S44" s="101"/>
-      <c r="T44" s="116"/>
-      <c r="U44" s="128"/>
-      <c r="V44" s="50"/>
-      <c r="W44" s="130"/>
+      <c r="K44" s="153"/>
+      <c r="L44" s="153"/>
+      <c r="M44" s="153"/>
+      <c r="N44" s="154"/>
+      <c r="O44" s="154"/>
+      <c r="P44" s="154"/>
+      <c r="Q44" s="154"/>
+      <c r="R44" s="154"/>
+      <c r="S44" s="154"/>
+      <c r="T44" s="192"/>
+      <c r="U44" s="156"/>
+      <c r="V44" s="47"/>
+      <c r="W44" s="159"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
@@ -4663,11 +4656,11 @@
       <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL44" s="123"/>
-      <c r="AM44" s="124"/>
-      <c r="AN44" s="125"/>
+        <v>41</v>
+      </c>
+      <c r="AL44" s="147"/>
+      <c r="AM44" s="148"/>
+      <c r="AN44" s="149"/>
       <c r="AO44" s="1"/>
       <c r="AP44" s="1"/>
       <c r="AQ44" s="1"/>
@@ -4677,7 +4670,7 @@
       <c r="A45" s="1">
         <v>500</v>
       </c>
-      <c r="B45" s="95"/>
+      <c r="B45" s="204"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -4686,31 +4679,31 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="7"/>
-      <c r="K45" s="101"/>
-      <c r="L45" s="101"/>
-      <c r="M45" s="102"/>
+      <c r="K45" s="154"/>
+      <c r="L45" s="154"/>
+      <c r="M45" s="205"/>
       <c r="N45" s="32"/>
-      <c r="O45" s="132" t="s">
-        <v>118</v>
-      </c>
-      <c r="P45" s="132" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q45" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="R45" s="132" t="s">
-        <v>121</v>
-      </c>
-      <c r="S45" s="132" t="s">
-        <v>122</v>
-      </c>
-      <c r="T45" s="135" t="s">
-        <v>123</v>
-      </c>
-      <c r="U45" s="128"/>
-      <c r="V45" s="50"/>
-      <c r="W45" s="130"/>
+      <c r="O45" s="161" t="s">
+        <v>187</v>
+      </c>
+      <c r="P45" s="161" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q45" s="161" t="s">
+        <v>111</v>
+      </c>
+      <c r="R45" s="161" t="s">
+        <v>112</v>
+      </c>
+      <c r="S45" s="161" t="s">
+        <v>113</v>
+      </c>
+      <c r="T45" s="164" t="s">
+        <v>114</v>
+      </c>
+      <c r="U45" s="156"/>
+      <c r="V45" s="47"/>
+      <c r="W45" s="159"/>
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
@@ -4725,10 +4718,10 @@
       <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL45" s="137" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="AL45" s="166" t="s">
+        <v>43</v>
       </c>
       <c r="AM45" s="1"/>
       <c r="AN45" s="1"/>
@@ -4741,8 +4734,8 @@
       <c r="A46" s="1">
         <v>600</v>
       </c>
-      <c r="B46" s="140" t="s">
-        <v>55</v>
+      <c r="B46" s="100" t="s">
+        <v>53</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -4750,29 +4743,29 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="143" t="s">
-        <v>124</v>
+      <c r="I46" s="103" t="s">
+        <v>115</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="146" t="s">
-        <v>125</v>
+      <c r="L46" s="106" t="s">
+        <v>116</v>
       </c>
       <c r="M46" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="N46" s="148" t="s">
-        <v>127</v>
-      </c>
-      <c r="O46" s="133"/>
-      <c r="P46" s="133"/>
-      <c r="Q46" s="133"/>
-      <c r="R46" s="134"/>
-      <c r="S46" s="134"/>
-      <c r="T46" s="136"/>
-      <c r="U46" s="128"/>
-      <c r="V46" s="50"/>
-      <c r="W46" s="130"/>
+        <v>117</v>
+      </c>
+      <c r="N46" s="108" t="s">
+        <v>118</v>
+      </c>
+      <c r="O46" s="162"/>
+      <c r="P46" s="162"/>
+      <c r="Q46" s="162"/>
+      <c r="R46" s="163"/>
+      <c r="S46" s="163"/>
+      <c r="T46" s="165"/>
+      <c r="U46" s="156"/>
+      <c r="V46" s="47"/>
+      <c r="W46" s="159"/>
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
@@ -4787,7 +4780,7 @@
       <c r="AI46" s="1"/>
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
-      <c r="AL46" s="138"/>
+      <c r="AL46" s="167"/>
       <c r="AM46" s="1"/>
       <c r="AN46" s="1"/>
       <c r="AO46" s="1"/>
@@ -4799,40 +4792,40 @@
       <c r="A47" s="1">
         <v>700</v>
       </c>
-      <c r="B47" s="141"/>
+      <c r="B47" s="101"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="144"/>
+      <c r="I47" s="104"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="150" t="s">
-        <v>128</v>
-      </c>
-      <c r="L47" s="147"/>
+      <c r="K47" s="110" t="s">
+        <v>119</v>
+      </c>
+      <c r="L47" s="107"/>
       <c r="M47" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="N47" s="149"/>
-      <c r="O47" s="133"/>
-      <c r="P47" s="133"/>
-      <c r="Q47" s="133"/>
+        <v>120</v>
+      </c>
+      <c r="N47" s="109"/>
+      <c r="O47" s="162"/>
+      <c r="P47" s="162"/>
+      <c r="Q47" s="162"/>
       <c r="R47" s="29" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="S47" s="29" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="T47" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="U47" s="129"/>
+        <v>123</v>
+      </c>
+      <c r="U47" s="157"/>
       <c r="V47" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="W47" s="131"/>
+        <v>124</v>
+      </c>
+      <c r="W47" s="160"/>
       <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
@@ -4847,7 +4840,7 @@
       <c r="AI47" s="1"/>
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
-      <c r="AL47" s="138"/>
+      <c r="AL47" s="167"/>
       <c r="AM47" s="1"/>
       <c r="AN47" s="1"/>
       <c r="AO47" s="1"/>
@@ -4859,32 +4852,32 @@
       <c r="A48" s="1">
         <v>800</v>
       </c>
-      <c r="B48" s="141"/>
+      <c r="B48" s="101"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="145"/>
+      <c r="I48" s="105"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="151"/>
+      <c r="K48" s="111"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="133"/>
-      <c r="P48" s="133"/>
-      <c r="Q48" s="133"/>
-      <c r="R48" s="153" t="s">
-        <v>134</v>
-      </c>
-      <c r="S48" s="156" t="s">
-        <v>135</v>
-      </c>
-      <c r="T48" s="157"/>
-      <c r="U48" s="157"/>
-      <c r="V48" s="157"/>
-      <c r="W48" s="158"/>
+      <c r="N48" s="235"/>
+      <c r="O48" s="163"/>
+      <c r="P48" s="162"/>
+      <c r="Q48" s="162"/>
+      <c r="R48" s="169" t="s">
+        <v>125</v>
+      </c>
+      <c r="S48" s="172" t="s">
+        <v>126</v>
+      </c>
+      <c r="T48" s="173"/>
+      <c r="U48" s="173"/>
+      <c r="V48" s="173"/>
+      <c r="W48" s="174"/>
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
@@ -4899,7 +4892,7 @@
       <c r="AI48" s="1"/>
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
-      <c r="AL48" s="138"/>
+      <c r="AL48" s="167"/>
       <c r="AM48" s="1"/>
       <c r="AN48" s="1"/>
       <c r="AO48" s="1"/>
@@ -4911,39 +4904,45 @@
       <c r="A49" s="1">
         <v>900</v>
       </c>
-      <c r="B49" s="141"/>
+      <c r="B49" s="101"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="159" t="s">
-        <v>136</v>
+      <c r="D49" s="112" t="s">
+        <v>127</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="184" t="s">
-        <v>137</v>
+      <c r="G49" s="125" t="s">
+        <v>128</v>
       </c>
       <c r="H49" s="1"/>
-      <c r="I49" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="J49" s="1"/>
-      <c r="K49" s="152"/>
+      <c r="I49" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="J49" s="238" t="s">
+        <v>190</v>
+      </c>
+      <c r="K49" s="237"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="O49" s="133"/>
-      <c r="P49" s="133"/>
-      <c r="Q49" s="133"/>
-      <c r="R49" s="154"/>
+      <c r="O49" s="236" t="s">
+        <v>188</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q49" s="162"/>
+      <c r="R49" s="170"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
-      <c r="U49" s="187" t="s">
-        <v>139</v>
-      </c>
-      <c r="V49" s="189" t="s">
-        <v>140</v>
-      </c>
-      <c r="W49" s="36" t="s">
-        <v>141</v>
+      <c r="U49" s="175" t="s">
+        <v>130</v>
+      </c>
+      <c r="V49" s="176" t="s">
+        <v>131</v>
+      </c>
+      <c r="W49" s="35" t="s">
+        <v>132</v>
       </c>
       <c r="X49" s="1"/>
       <c r="Y49" s="1"/>
@@ -4959,7 +4958,7 @@
       <c r="AI49" s="1"/>
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
-      <c r="AL49" s="138"/>
+      <c r="AL49" s="167"/>
       <c r="AM49" s="1"/>
       <c r="AN49" s="1"/>
       <c r="AO49" s="1"/>
@@ -4971,35 +4970,35 @@
       <c r="A50" s="1">
         <v>1000</v>
       </c>
-      <c r="B50" s="141"/>
+      <c r="B50" s="101"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="160"/>
-      <c r="E50" s="162" t="s">
-        <v>142</v>
+      <c r="D50" s="113"/>
+      <c r="E50" s="115" t="s">
+        <v>133</v>
       </c>
       <c r="F50" s="1"/>
-      <c r="G50" s="185"/>
-      <c r="H50" s="165" t="s">
-        <v>143</v>
+      <c r="G50" s="126"/>
+      <c r="H50" s="89" t="s">
+        <v>134</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="19" t="s">
-        <v>144</v>
+        <v>189</v>
       </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-      <c r="O50" s="133"/>
-      <c r="P50" s="133"/>
-      <c r="Q50" s="133"/>
-      <c r="R50" s="154"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="162"/>
+      <c r="R50" s="170"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
-      <c r="U50" s="188"/>
-      <c r="V50" s="190"/>
+      <c r="U50" s="83"/>
+      <c r="V50" s="177"/>
       <c r="W50" s="16" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="X50" s="1"/>
       <c r="Y50" s="1"/>
@@ -5015,7 +5014,7 @@
       <c r="AI50" s="1"/>
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
-      <c r="AL50" s="138"/>
+      <c r="AL50" s="167"/>
       <c r="AM50" s="1"/>
       <c r="AN50" s="1"/>
       <c r="AO50" s="1"/>
@@ -5027,39 +5026,43 @@
       <c r="A51" s="1">
         <v>1100</v>
       </c>
-      <c r="B51" s="141"/>
+      <c r="B51" s="101"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="160"/>
-      <c r="E51" s="163"/>
+      <c r="D51" s="113"/>
+      <c r="E51" s="116"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="186"/>
-      <c r="H51" s="166"/>
+      <c r="G51" s="127"/>
+      <c r="H51" s="118"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="168" t="s">
-        <v>146</v>
-      </c>
-      <c r="K51" s="171" t="s">
-        <v>147</v>
+      <c r="J51" s="119" t="s">
+        <v>136</v>
+      </c>
+      <c r="K51" s="122" t="s">
+        <v>137</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
-      <c r="O51" s="133"/>
-      <c r="P51" s="133"/>
-      <c r="Q51" s="133"/>
-      <c r="R51" s="155"/>
+      <c r="O51" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="P51" s="108" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q51" s="162"/>
+      <c r="R51" s="171"/>
       <c r="S51" s="1"/>
-      <c r="T51" s="37" t="s">
-        <v>148</v>
-      </c>
-      <c r="U51" s="38" t="s">
-        <v>149</v>
+      <c r="T51" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="U51" s="37" t="s">
+        <v>139</v>
       </c>
       <c r="V51" s="22" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="W51" s="16" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="X51" s="1"/>
       <c r="Y51" s="1"/>
@@ -5074,10 +5077,10 @@
       <c r="AH51" s="1"/>
       <c r="AI51" s="1"/>
       <c r="AJ51" s="1"/>
-      <c r="AK51" s="207" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL51" s="138"/>
+      <c r="AK51" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL51" s="167"/>
       <c r="AM51" s="1"/>
       <c r="AN51" s="1"/>
       <c r="AO51" s="1"/>
@@ -5089,32 +5092,32 @@
       <c r="A52" s="1">
         <v>1200</v>
       </c>
-      <c r="B52" s="141"/>
+      <c r="B52" s="101"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="160"/>
-      <c r="E52" s="163"/>
+      <c r="D52" s="113"/>
+      <c r="E52" s="116"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="166"/>
+      <c r="H52" s="118"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="169"/>
-      <c r="K52" s="172"/>
+      <c r="J52" s="120"/>
+      <c r="K52" s="123"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
-      <c r="O52" s="134"/>
-      <c r="P52" s="134"/>
-      <c r="Q52" s="133"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="109"/>
+      <c r="Q52" s="162"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="25" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="W52" s="1"/>
       <c r="X52" s="16" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
@@ -5127,11 +5130,11 @@
       <c r="AG52" s="1"/>
       <c r="AH52" s="1"/>
       <c r="AI52" s="1"/>
-      <c r="AJ52" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK52" s="208"/>
-      <c r="AL52" s="138"/>
+      <c r="AJ52" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK52" s="74"/>
+      <c r="AL52" s="167"/>
       <c r="AM52" s="1"/>
       <c r="AN52" s="1"/>
       <c r="AO52" s="1"/>
@@ -5143,42 +5146,42 @@
       <c r="A53" s="1">
         <v>1300</v>
       </c>
-      <c r="B53" s="141"/>
-      <c r="C53" s="210" t="s">
-        <v>154</v>
-      </c>
-      <c r="D53" s="160"/>
-      <c r="E53" s="163"/>
+      <c r="B53" s="101"/>
+      <c r="C53" s="134" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="113"/>
+      <c r="E53" s="116"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="H53" s="166"/>
+      <c r="G53" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="H53" s="118"/>
       <c r="I53" s="1"/>
-      <c r="J53" s="169"/>
-      <c r="K53" s="172"/>
+      <c r="J53" s="120"/>
+      <c r="K53" s="123"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
-      <c r="Q53" s="133"/>
+      <c r="Q53" s="162"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
       <c r="T53" s="16" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="U53" s="16" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="V53" s="25" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="W53" s="16" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="X53" s="16" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
@@ -5191,9 +5194,9 @@
       <c r="AG53" s="1"/>
       <c r="AH53" s="1"/>
       <c r="AI53" s="1"/>
-      <c r="AJ53" s="52"/>
-      <c r="AK53" s="208"/>
-      <c r="AL53" s="138"/>
+      <c r="AJ53" s="77"/>
+      <c r="AK53" s="74"/>
+      <c r="AL53" s="167"/>
       <c r="AM53" s="1"/>
       <c r="AN53" s="1"/>
       <c r="AO53" s="1"/>
@@ -5205,39 +5208,39 @@
       <c r="A54" s="1">
         <v>1400</v>
       </c>
-      <c r="B54" s="142"/>
-      <c r="C54" s="211"/>
-      <c r="D54" s="160"/>
-      <c r="E54" s="163"/>
+      <c r="B54" s="102"/>
+      <c r="C54" s="135"/>
+      <c r="D54" s="113"/>
+      <c r="E54" s="116"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="213" t="s">
-        <v>161</v>
-      </c>
-      <c r="H54" s="167"/>
+      <c r="G54" s="79" t="s">
+        <v>151</v>
+      </c>
+      <c r="H54" s="90"/>
       <c r="I54" s="1"/>
-      <c r="J54" s="169"/>
-      <c r="K54" s="172"/>
+      <c r="J54" s="120"/>
+      <c r="K54" s="123"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
-      <c r="Q54" s="133"/>
+      <c r="Q54" s="162"/>
       <c r="R54" s="1"/>
-      <c r="S54" s="215" t="s">
-        <v>162</v>
-      </c>
-      <c r="T54" s="216"/>
+      <c r="S54" s="81" t="s">
+        <v>152</v>
+      </c>
+      <c r="T54" s="82"/>
       <c r="U54" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="V54" s="218" t="s">
-        <v>164</v>
-      </c>
-      <c r="W54" s="179" t="s">
-        <v>165</v>
-      </c>
-      <c r="X54" s="180"/>
+        <v>153</v>
+      </c>
+      <c r="V54" s="85" t="s">
+        <v>154</v>
+      </c>
+      <c r="W54" s="98" t="s">
+        <v>155</v>
+      </c>
+      <c r="X54" s="99"/>
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
@@ -5249,9 +5252,9 @@
       <c r="AG54" s="1"/>
       <c r="AH54" s="1"/>
       <c r="AI54" s="1"/>
-      <c r="AJ54" s="52"/>
-      <c r="AK54" s="208"/>
-      <c r="AL54" s="139"/>
+      <c r="AJ54" s="77"/>
+      <c r="AK54" s="74"/>
+      <c r="AL54" s="168"/>
       <c r="AM54" s="1"/>
       <c r="AN54" s="1"/>
       <c r="AO54" s="1"/>
@@ -5263,39 +5266,39 @@
       <c r="A55" s="1">
         <v>1500</v>
       </c>
-      <c r="B55" s="191" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="211"/>
-      <c r="D55" s="160"/>
-      <c r="E55" s="163"/>
+      <c r="B55" s="128" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="135"/>
+      <c r="D55" s="113"/>
+      <c r="E55" s="116"/>
       <c r="F55" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="G55" s="214"/>
-      <c r="H55" s="194" t="s">
-        <v>167</v>
+        <v>156</v>
+      </c>
+      <c r="G55" s="80"/>
+      <c r="H55" s="131" t="s">
+        <v>157</v>
       </c>
       <c r="I55" s="1"/>
-      <c r="J55" s="169"/>
-      <c r="K55" s="172"/>
+      <c r="J55" s="120"/>
+      <c r="K55" s="123"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
-      <c r="P55" s="181" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q55" s="134"/>
-      <c r="R55" s="181" t="s">
-        <v>169</v>
-      </c>
-      <c r="S55" s="188"/>
-      <c r="T55" s="217"/>
+      <c r="P55" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q55" s="163"/>
+      <c r="R55" s="70" t="s">
+        <v>159</v>
+      </c>
+      <c r="S55" s="83"/>
+      <c r="T55" s="84"/>
       <c r="U55" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="V55" s="219"/>
+        <v>160</v>
+      </c>
+      <c r="V55" s="86"/>
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
       <c r="Y55" s="1"/>
@@ -5309,10 +5312,10 @@
       <c r="AG55" s="1"/>
       <c r="AH55" s="1"/>
       <c r="AI55" s="1"/>
-      <c r="AJ55" s="52"/>
-      <c r="AK55" s="208"/>
-      <c r="AL55" s="197" t="s">
-        <v>48</v>
+      <c r="AJ55" s="77"/>
+      <c r="AK55" s="74"/>
+      <c r="AL55" s="60" t="s">
+        <v>46</v>
       </c>
       <c r="AM55" s="1"/>
       <c r="AN55" s="1"/>
@@ -5325,44 +5328,44 @@
       <c r="A56" s="1">
         <v>1600</v>
       </c>
-      <c r="B56" s="192"/>
-      <c r="C56" s="211"/>
-      <c r="D56" s="161"/>
-      <c r="E56" s="163"/>
+      <c r="B56" s="129"/>
+      <c r="C56" s="135"/>
+      <c r="D56" s="114"/>
+      <c r="E56" s="116"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="199" t="s">
-        <v>171</v>
-      </c>
-      <c r="H56" s="195"/>
-      <c r="I56" s="202" t="s">
-        <v>172</v>
-      </c>
-      <c r="J56" s="170"/>
-      <c r="K56" s="172"/>
-      <c r="L56" s="204" t="s">
-        <v>173</v>
+      <c r="G56" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="H56" s="132"/>
+      <c r="I56" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="J56" s="121"/>
+      <c r="K56" s="123"/>
+      <c r="L56" s="67" t="s">
+        <v>163</v>
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
-      <c r="O56" s="181" t="s">
-        <v>174</v>
-      </c>
-      <c r="P56" s="182"/>
-      <c r="Q56" s="181" t="s">
-        <v>175</v>
-      </c>
-      <c r="R56" s="182"/>
-      <c r="S56" s="181" t="s">
-        <v>176</v>
-      </c>
-      <c r="T56" s="181" t="s">
-        <v>177</v>
-      </c>
-      <c r="U56" s="181" t="s">
-        <v>178</v>
-      </c>
-      <c r="V56" s="174" t="s">
-        <v>179</v>
+      <c r="O56" s="70" t="s">
+        <v>191</v>
+      </c>
+      <c r="P56" s="71"/>
+      <c r="Q56" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="R56" s="71"/>
+      <c r="S56" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="T56" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="U56" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="V56" s="93" t="s">
+        <v>168</v>
       </c>
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
@@ -5377,9 +5380,9 @@
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
       <c r="AI56" s="1"/>
-      <c r="AJ56" s="52"/>
-      <c r="AK56" s="208"/>
-      <c r="AL56" s="198"/>
+      <c r="AJ56" s="77"/>
+      <c r="AK56" s="74"/>
+      <c r="AL56" s="61"/>
       <c r="AM56" s="1"/>
       <c r="AN56" s="1"/>
       <c r="AO56" s="1"/>
@@ -5391,31 +5394,31 @@
       <c r="A57" s="1">
         <v>1700</v>
       </c>
-      <c r="B57" s="193"/>
-      <c r="C57" s="212"/>
-      <c r="D57" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="E57" s="164"/>
+      <c r="B57" s="130"/>
+      <c r="C57" s="136"/>
+      <c r="D57" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="E57" s="117"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="200"/>
-      <c r="H57" s="195"/>
-      <c r="I57" s="203"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="132"/>
+      <c r="I57" s="66"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="172"/>
-      <c r="L57" s="205"/>
+      <c r="K57" s="123"/>
+      <c r="L57" s="68"/>
       <c r="M57" s="1"/>
-      <c r="N57" s="177" t="s">
-        <v>181</v>
-      </c>
-      <c r="O57" s="182"/>
-      <c r="P57" s="182"/>
-      <c r="Q57" s="182"/>
-      <c r="R57" s="182"/>
-      <c r="S57" s="182"/>
-      <c r="T57" s="182"/>
-      <c r="U57" s="182"/>
-      <c r="V57" s="175"/>
+      <c r="N57" s="96" t="s">
+        <v>170</v>
+      </c>
+      <c r="O57" s="71"/>
+      <c r="P57" s="71"/>
+      <c r="Q57" s="71"/>
+      <c r="R57" s="71"/>
+      <c r="S57" s="71"/>
+      <c r="T57" s="71"/>
+      <c r="U57" s="71"/>
+      <c r="V57" s="94"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
@@ -5429,10 +5432,10 @@
       <c r="AG57" s="1"/>
       <c r="AH57" s="1"/>
       <c r="AI57" s="1"/>
-      <c r="AJ57" s="52"/>
-      <c r="AK57" s="208"/>
+      <c r="AJ57" s="77"/>
+      <c r="AK57" s="74"/>
       <c r="AL57" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AM57" s="1"/>
       <c r="AN57" s="1"/>
@@ -5446,32 +5449,32 @@
         <v>1800</v>
       </c>
       <c r="B58" s="1"/>
-      <c r="C58" s="226" t="s">
-        <v>182</v>
-      </c>
-      <c r="D58" s="228" t="s">
-        <v>183</v>
-      </c>
-      <c r="E58" s="229"/>
+      <c r="C58" s="139" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="E58" s="49"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="200"/>
-      <c r="H58" s="196"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="133"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="172"/>
-      <c r="L58" s="205"/>
-      <c r="M58" s="234" t="s">
-        <v>184</v>
-      </c>
-      <c r="N58" s="178"/>
-      <c r="O58" s="183"/>
-      <c r="P58" s="182"/>
-      <c r="Q58" s="182"/>
-      <c r="R58" s="182"/>
-      <c r="S58" s="182"/>
-      <c r="T58" s="182"/>
-      <c r="U58" s="182"/>
-      <c r="V58" s="175"/>
+      <c r="K58" s="123"/>
+      <c r="L58" s="68"/>
+      <c r="M58" s="54" t="s">
+        <v>173</v>
+      </c>
+      <c r="N58" s="97"/>
+      <c r="O58" s="71"/>
+      <c r="P58" s="71"/>
+      <c r="Q58" s="71"/>
+      <c r="R58" s="71"/>
+      <c r="S58" s="71"/>
+      <c r="T58" s="71"/>
+      <c r="U58" s="71"/>
+      <c r="V58" s="94"/>
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
       <c r="Y58" s="1"/>
@@ -5485,10 +5488,10 @@
       <c r="AG58" s="1"/>
       <c r="AH58" s="1"/>
       <c r="AI58" s="1"/>
-      <c r="AJ58" s="52"/>
-      <c r="AK58" s="209"/>
+      <c r="AJ58" s="77"/>
+      <c r="AK58" s="75"/>
       <c r="AL58" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AM58" s="1"/>
       <c r="AN58" s="1"/>
@@ -5502,34 +5505,32 @@
         <v>1900</v>
       </c>
       <c r="B59" s="1"/>
-      <c r="C59" s="227"/>
-      <c r="D59" s="230"/>
-      <c r="E59" s="231"/>
-      <c r="F59" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="G59" s="200"/>
+      <c r="C59" s="140"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G59" s="63"/>
       <c r="H59" s="21" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="I59" s="1"/>
-      <c r="J59" s="237" t="s">
-        <v>187</v>
-      </c>
-      <c r="K59" s="172"/>
-      <c r="L59" s="205"/>
-      <c r="M59" s="235"/>
+      <c r="J59" s="57" t="s">
+        <v>176</v>
+      </c>
+      <c r="K59" s="123"/>
+      <c r="L59" s="68"/>
+      <c r="M59" s="55"/>
       <c r="N59" s="1"/>
-      <c r="O59" s="240" t="s">
-        <v>188</v>
-      </c>
-      <c r="P59" s="183"/>
-      <c r="Q59" s="183"/>
-      <c r="R59" s="183"/>
-      <c r="S59" s="183"/>
-      <c r="T59" s="183"/>
-      <c r="U59" s="183"/>
-      <c r="V59" s="176"/>
+      <c r="O59" s="71"/>
+      <c r="P59" s="72"/>
+      <c r="Q59" s="72"/>
+      <c r="R59" s="72"/>
+      <c r="S59" s="72"/>
+      <c r="T59" s="72"/>
+      <c r="U59" s="72"/>
+      <c r="V59" s="95"/>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
       <c r="Y59" s="1"/>
@@ -5543,11 +5544,11 @@
       <c r="AG59" s="1"/>
       <c r="AH59" s="1"/>
       <c r="AI59" s="1"/>
-      <c r="AJ59" s="52"/>
-      <c r="AK59" s="220" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL59" s="221"/>
+      <c r="AJ59" s="77"/>
+      <c r="AK59" s="87" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL59" s="88"/>
       <c r="AM59" s="1"/>
       <c r="AN59" s="1"/>
       <c r="AO59" s="1"/>
@@ -5560,25 +5561,27 @@
         <v>2000</v>
       </c>
       <c r="B60" s="1"/>
-      <c r="C60" s="222" t="s">
-        <v>189</v>
-      </c>
-      <c r="D60" s="230"/>
-      <c r="E60" s="231"/>
+      <c r="C60" s="137" t="s">
+        <v>177</v>
+      </c>
+      <c r="D60" s="50"/>
+      <c r="E60" s="51"/>
       <c r="F60" s="1"/>
-      <c r="G60" s="200"/>
-      <c r="H60" s="165" t="s">
-        <v>190</v>
-      </c>
-      <c r="I60" s="224" t="s">
-        <v>191</v>
-      </c>
-      <c r="J60" s="238"/>
-      <c r="K60" s="172"/>
-      <c r="L60" s="205"/>
-      <c r="M60" s="235"/>
+      <c r="G60" s="63"/>
+      <c r="H60" s="89" t="s">
+        <v>178</v>
+      </c>
+      <c r="I60" s="91" t="s">
+        <v>179</v>
+      </c>
+      <c r="J60" s="58"/>
+      <c r="K60" s="123"/>
+      <c r="L60" s="68"/>
+      <c r="M60" s="55"/>
       <c r="N60" s="1"/>
-      <c r="O60" s="241"/>
+      <c r="O60" s="22" t="s">
+        <v>192</v>
+      </c>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -5598,11 +5601,11 @@
       <c r="AG60" s="1"/>
       <c r="AH60" s="1"/>
       <c r="AI60" s="1"/>
-      <c r="AJ60" s="52"/>
-      <c r="AK60" s="207" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL60" s="197"/>
+      <c r="AJ60" s="77"/>
+      <c r="AK60" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL60" s="60"/>
       <c r="AM60" s="1"/>
       <c r="AN60" s="1"/>
       <c r="AO60" s="1"/>
@@ -5615,19 +5618,18 @@
         <v>2100</v>
       </c>
       <c r="B61" s="1"/>
-      <c r="C61" s="223"/>
-      <c r="D61" s="232"/>
-      <c r="E61" s="233"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="52"/>
+      <c r="E61" s="53"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="201"/>
-      <c r="H61" s="167"/>
-      <c r="I61" s="225"/>
-      <c r="J61" s="239"/>
-      <c r="K61" s="173"/>
-      <c r="L61" s="206"/>
-      <c r="M61" s="236"/>
+      <c r="G61" s="64"/>
+      <c r="H61" s="90"/>
+      <c r="I61" s="92"/>
+      <c r="J61" s="59"/>
+      <c r="K61" s="124"/>
+      <c r="L61" s="69"/>
+      <c r="M61" s="56"/>
       <c r="N61" s="1"/>
-      <c r="O61" s="242"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -5647,9 +5649,9 @@
       <c r="AG61" s="1"/>
       <c r="AH61" s="1"/>
       <c r="AI61" s="1"/>
-      <c r="AJ61" s="53"/>
-      <c r="AK61" s="209"/>
-      <c r="AL61" s="198"/>
+      <c r="AJ61" s="78"/>
+      <c r="AK61" s="75"/>
+      <c r="AL61" s="61"/>
       <c r="AM61" s="1"/>
       <c r="AN61" s="1"/>
       <c r="AO61" s="1"/>
@@ -5659,33 +5661,60 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="D58:E61"/>
-    <mergeCell ref="M58:M61"/>
-    <mergeCell ref="J59:J61"/>
-    <mergeCell ref="O59:O61"/>
-    <mergeCell ref="AL55:AL56"/>
-    <mergeCell ref="G56:G61"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="L56:L61"/>
-    <mergeCell ref="O56:O58"/>
-    <mergeCell ref="Q56:Q59"/>
-    <mergeCell ref="AK51:AK58"/>
-    <mergeCell ref="AJ52:AJ61"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="S54:T55"/>
-    <mergeCell ref="V54:V55"/>
-    <mergeCell ref="AK59:AL59"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="AK60:AL61"/>
-    <mergeCell ref="V56:V59"/>
-    <mergeCell ref="N57:N58"/>
-    <mergeCell ref="W54:X54"/>
-    <mergeCell ref="S56:S59"/>
-    <mergeCell ref="T56:T59"/>
-    <mergeCell ref="U56:U59"/>
-    <mergeCell ref="P55:P59"/>
-    <mergeCell ref="R55:R59"/>
+    <mergeCell ref="O56:O59"/>
+    <mergeCell ref="P40:P44"/>
+    <mergeCell ref="P45:P48"/>
+    <mergeCell ref="P51:P52"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="U2:U17"/>
+    <mergeCell ref="B7:B28"/>
+    <mergeCell ref="S9:S14"/>
+    <mergeCell ref="S15:S18"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="S20:S24"/>
+    <mergeCell ref="U21:U22"/>
+    <mergeCell ref="R24:R28"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="S26:S30"/>
+    <mergeCell ref="T26:T28"/>
+    <mergeCell ref="B29:B35"/>
+    <mergeCell ref="R29:R33"/>
+    <mergeCell ref="S31:S33"/>
+    <mergeCell ref="M33:M35"/>
+    <mergeCell ref="U33:U34"/>
+    <mergeCell ref="N34:N38"/>
+    <mergeCell ref="Q34:R35"/>
+    <mergeCell ref="B36:B45"/>
+    <mergeCell ref="M36:M40"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="K40:K45"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="N41:N44"/>
+    <mergeCell ref="S41:S44"/>
+    <mergeCell ref="O45:O48"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="S38:S40"/>
+    <mergeCell ref="U38:U39"/>
+    <mergeCell ref="L39:L45"/>
+    <mergeCell ref="O39:O44"/>
+    <mergeCell ref="W39:W42"/>
+    <mergeCell ref="Q40:R44"/>
+    <mergeCell ref="T40:T44"/>
+    <mergeCell ref="U40:U42"/>
+    <mergeCell ref="AL41:AN44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="U43:U47"/>
+    <mergeCell ref="W43:W47"/>
+    <mergeCell ref="Q45:Q55"/>
+    <mergeCell ref="R45:R46"/>
+    <mergeCell ref="S45:S46"/>
+    <mergeCell ref="T45:T46"/>
+    <mergeCell ref="AL45:AL54"/>
+    <mergeCell ref="R48:R51"/>
+    <mergeCell ref="S48:W48"/>
+    <mergeCell ref="U49:U50"/>
+    <mergeCell ref="V49:V50"/>
     <mergeCell ref="B46:B54"/>
     <mergeCell ref="I46:I48"/>
     <mergeCell ref="L46:L47"/>
@@ -5702,59 +5731,33 @@
     <mergeCell ref="C53:C57"/>
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="C58:C59"/>
-    <mergeCell ref="AL41:AN44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="P42:P44"/>
-    <mergeCell ref="U43:U47"/>
-    <mergeCell ref="W43:W47"/>
-    <mergeCell ref="O45:O52"/>
-    <mergeCell ref="P45:P52"/>
-    <mergeCell ref="Q45:Q55"/>
-    <mergeCell ref="R45:R46"/>
-    <mergeCell ref="S45:S46"/>
-    <mergeCell ref="T45:T46"/>
-    <mergeCell ref="AL45:AL54"/>
-    <mergeCell ref="R48:R51"/>
-    <mergeCell ref="S48:W48"/>
-    <mergeCell ref="U49:U50"/>
-    <mergeCell ref="V49:V50"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="S38:S40"/>
-    <mergeCell ref="U38:U39"/>
-    <mergeCell ref="L39:L45"/>
-    <mergeCell ref="O39:O44"/>
-    <mergeCell ref="W39:W42"/>
-    <mergeCell ref="Q40:R44"/>
-    <mergeCell ref="T40:T44"/>
-    <mergeCell ref="U40:U42"/>
-    <mergeCell ref="U33:U34"/>
-    <mergeCell ref="N34:N38"/>
-    <mergeCell ref="Q34:R35"/>
-    <mergeCell ref="B36:B45"/>
-    <mergeCell ref="M36:M40"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="K40:K45"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="N41:N44"/>
-    <mergeCell ref="S41:S44"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="U2:U17"/>
-    <mergeCell ref="B7:B28"/>
-    <mergeCell ref="S9:S14"/>
-    <mergeCell ref="S15:S18"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="S20:S24"/>
-    <mergeCell ref="U21:U22"/>
-    <mergeCell ref="R24:R28"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="S26:S30"/>
-    <mergeCell ref="T26:T28"/>
-    <mergeCell ref="B29:B35"/>
-    <mergeCell ref="R29:R33"/>
-    <mergeCell ref="S31:S33"/>
-    <mergeCell ref="M33:M35"/>
+    <mergeCell ref="W54:X54"/>
+    <mergeCell ref="S56:S59"/>
+    <mergeCell ref="T56:T59"/>
+    <mergeCell ref="U56:U59"/>
+    <mergeCell ref="P55:P59"/>
+    <mergeCell ref="R55:R59"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="AK60:AL61"/>
+    <mergeCell ref="V56:V59"/>
+    <mergeCell ref="N57:N58"/>
+    <mergeCell ref="D58:E61"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="J59:J61"/>
+    <mergeCell ref="AL55:AL56"/>
+    <mergeCell ref="G56:G61"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="L56:L61"/>
+    <mergeCell ref="Q56:Q59"/>
+    <mergeCell ref="AK51:AK58"/>
+    <mergeCell ref="AJ52:AJ61"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="S54:T55"/>
+    <mergeCell ref="V54:V55"/>
+    <mergeCell ref="AK59:AL59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>